<commit_message>
Update our data to include BP 2022 data
</commit_message>
<xml_diff>
--- a/data/Germany & Spain Data.xlsx
+++ b/data/Germany & Spain Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trtim/Develop/germany-and-spain/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF5364B-7D66-2447-AFA0-AB98B502B469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA57CFB8-6615-5442-B1B6-FF0C99AE94C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FE379562-162F-468A-B10D-43820705E65E}"/>
+    <workbookView xWindow="0" yWindow="10640" windowWidth="33720" windowHeight="10960" activeTab="3" xr2:uid="{FE379562-162F-468A-B10D-43820705E65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="5" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={65BC9C15-FA43-411D-BC1F-A5AB6869904D}</author>
-    <author>tc={136236B7-1BD8-4BCF-9D25-04399D493AF0}</author>
-    <author>tc={9390F296-094A-4F9A-B338-01C2CA1B4623}</author>
     <author>tc={24E521ED-F1DA-4703-9D73-DA57634E0F5C}</author>
     <author>tc={35ACCA49-9A92-480D-9B62-B9A273372211}</author>
     <author>tc={92D421E6-7F5E-4E90-A4DE-1A0477DC08E4}</author>
@@ -49,31 +46,7 @@
     <author>tc={79D5ED60-DAD0-473C-8A58-27633F938CF7}</author>
   </authors>
   <commentList>
-    <comment ref="Y5" authorId="0" shapeId="0" xr:uid="{65BC9C15-FA43-411D-BC1F-A5AB6869904D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Preliminary data, -9.6% (AGEB)</t>
-      </text>
-    </comment>
-    <comment ref="Z5" authorId="1" shapeId="0" xr:uid="{136236B7-1BD8-4BCF-9D25-04399D493AF0}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Preliminary data +4.5% AGORA</t>
-      </text>
-    </comment>
-    <comment ref="Y6" authorId="2" shapeId="0" xr:uid="{9390F296-094A-4F9A-B338-01C2CA1B4623}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Preliminary data, -18.9% (BP)</t>
-      </text>
-    </comment>
-    <comment ref="Y10" authorId="3" shapeId="0" xr:uid="{24E521ED-F1DA-4703-9D73-DA57634E0F5C}">
+    <comment ref="Y10" authorId="0" shapeId="0" xr:uid="{24E521ED-F1DA-4703-9D73-DA57634E0F5C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -81,7 +54,7 @@
     Preliminary data, -8% (AGEB)</t>
       </text>
     </comment>
-    <comment ref="Z10" authorId="4" shapeId="0" xr:uid="{35ACCA49-9A92-480D-9B62-B9A273372211}">
+    <comment ref="Z10" authorId="1" shapeId="0" xr:uid="{35ACCA49-9A92-480D-9B62-B9A273372211}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -89,7 +62,7 @@
     Preliminary data +2.6% AGORA</t>
       </text>
     </comment>
-    <comment ref="Y11" authorId="5" shapeId="0" xr:uid="{92D421E6-7F5E-4E90-A4DE-1A0477DC08E4}">
+    <comment ref="Y11" authorId="2" shapeId="0" xr:uid="{92D421E6-7F5E-4E90-A4DE-1A0477DC08E4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -97,7 +70,7 @@
     Preliminary data, -11.4% (BP)</t>
       </text>
     </comment>
-    <comment ref="Y24" authorId="6" shapeId="0" xr:uid="{430E2E63-DEB6-4C79-B7B8-EB39157A1F7C}">
+    <comment ref="Y24" authorId="3" shapeId="0" xr:uid="{430E2E63-DEB6-4C79-B7B8-EB39157A1F7C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -105,7 +78,7 @@
     Populatin at the 01.01.2020, source Instituto Nacional de Estadistica (Espana), consulted at 03.02.2022</t>
       </text>
     </comment>
-    <comment ref="Z24" authorId="7" shapeId="0" xr:uid="{79D5ED60-DAD0-473C-8A58-27633F938CF7}">
+    <comment ref="Z24" authorId="4" shapeId="0" xr:uid="{79D5ED60-DAD0-473C-8A58-27633F938CF7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -438,13 +411,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -520,15 +494,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -560,16 +525,12 @@
     <xf numFmtId="165" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,9 +540,20 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 18" xfId="4" xr:uid="{06ACEDC1-5CC0-E442-87B3-98D4C02855F7}"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{05A62228-BAA6-46A3-88C0-5B6930D4B7CE}"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
     <cellStyle name="Standard 2" xfId="3" xr:uid="{629DA393-64FF-480E-B039-636939B18E9E}"/>
@@ -902,15 +874,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="Y5" dT="2022-03-02T14:42:33.96" personId="{68492306-10FA-499D-9276-5B029AC11004}" id="{65BC9C15-FA43-411D-BC1F-A5AB6869904D}">
-    <text>Preliminary data, -9.6% (AGEB)</text>
-  </threadedComment>
-  <threadedComment ref="Z5" dT="2022-03-02T14:43:01.09" personId="{68492306-10FA-499D-9276-5B029AC11004}" id="{136236B7-1BD8-4BCF-9D25-04399D493AF0}">
-    <text>Preliminary data +4.5% AGORA</text>
-  </threadedComment>
-  <threadedComment ref="Y6" dT="2022-03-02T14:42:33.96" personId="{68492306-10FA-499D-9276-5B029AC11004}" id="{9390F296-094A-4F9A-B338-01C2CA1B4623}">
-    <text>Preliminary data, -18.9% (BP)</text>
-  </threadedComment>
   <threadedComment ref="Y10" dT="2022-03-02T14:42:33.96" personId="{68492306-10FA-499D-9276-5B029AC11004}" id="{24E521ED-F1DA-4703-9D73-DA57634E0F5C}">
     <text>Preliminary data, -8% (AGEB)</text>
   </threadedComment>
@@ -933,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A318FC36-9A92-4E6E-ACE0-025499D7FA26}">
   <dimension ref="A3:AB24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:Z19"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -948,7 +911,7 @@
       <c r="A3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="28"/>
@@ -960,79 +923,79 @@
       <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="42">
         <v>1997</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="42">
         <v>1998</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="42">
         <v>1999</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="42">
         <v>2000</v>
       </c>
-      <c r="F4" s="47">
+      <c r="F4" s="42">
         <v>2001</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="42">
         <v>2002</v>
       </c>
-      <c r="H4" s="47">
+      <c r="H4" s="42">
         <v>2003</v>
       </c>
-      <c r="I4" s="47">
+      <c r="I4" s="42">
         <v>2004</v>
       </c>
-      <c r="J4" s="47">
+      <c r="J4" s="42">
         <v>2005</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="42">
         <v>2006</v>
       </c>
-      <c r="L4" s="47">
+      <c r="L4" s="42">
         <v>2007</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="42">
         <v>2008</v>
       </c>
-      <c r="N4" s="47">
+      <c r="N4" s="42">
         <v>2009</v>
       </c>
-      <c r="O4" s="47">
+      <c r="O4" s="42">
         <v>2010</v>
       </c>
-      <c r="P4" s="47">
+      <c r="P4" s="42">
         <v>2011</v>
       </c>
-      <c r="Q4" s="47">
+      <c r="Q4" s="42">
         <v>2012</v>
       </c>
-      <c r="R4" s="47">
+      <c r="R4" s="42">
         <v>2013</v>
       </c>
-      <c r="S4" s="47">
+      <c r="S4" s="42">
         <v>2014</v>
       </c>
-      <c r="T4" s="47">
+      <c r="T4" s="42">
         <v>2015</v>
       </c>
-      <c r="U4" s="47">
+      <c r="U4" s="42">
         <v>2016</v>
       </c>
-      <c r="V4" s="47">
+      <c r="V4" s="42">
         <v>2017</v>
       </c>
-      <c r="W4" s="48">
+      <c r="W4" s="43">
         <v>2018</v>
       </c>
-      <c r="X4" s="48">
+      <c r="X4" s="43">
         <v>2019</v>
       </c>
-      <c r="Y4" s="48">
+      <c r="Y4" s="43">
         <v>2020</v>
       </c>
-      <c r="Z4" s="34">
+      <c r="Z4" s="31">
         <v>2021</v>
       </c>
     </row>
@@ -1040,164 +1003,160 @@
       <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="25">
-        <v>931324.2</v>
-      </c>
-      <c r="C5" s="25">
-        <v>923356.69</v>
-      </c>
-      <c r="D5" s="25">
-        <v>895874.33</v>
-      </c>
-      <c r="E5" s="25">
-        <v>899852.06</v>
-      </c>
-      <c r="F5" s="25">
-        <v>916648.52</v>
-      </c>
-      <c r="G5" s="25">
-        <v>899971.4</v>
-      </c>
-      <c r="H5" s="25">
-        <v>901151.9</v>
-      </c>
-      <c r="I5" s="25">
-        <v>887089.13</v>
-      </c>
-      <c r="J5" s="25">
-        <v>866697.22</v>
-      </c>
-      <c r="K5" s="25">
-        <v>878320.43</v>
-      </c>
-      <c r="L5" s="25">
-        <v>851624.33</v>
-      </c>
-      <c r="M5" s="25">
-        <v>854927.15</v>
-      </c>
-      <c r="N5" s="25">
-        <v>790294.72</v>
-      </c>
-      <c r="O5" s="25">
-        <v>832949.11</v>
-      </c>
-      <c r="P5" s="25">
-        <v>809216.92</v>
-      </c>
-      <c r="Q5" s="25">
-        <v>813984.65</v>
-      </c>
-      <c r="R5" s="25">
-        <v>831453.84</v>
-      </c>
-      <c r="S5" s="25">
-        <v>792587.77</v>
-      </c>
-      <c r="T5" s="25">
-        <v>795610.21</v>
-      </c>
-      <c r="U5" s="25">
-        <v>800686.63</v>
-      </c>
-      <c r="V5" s="25">
-        <v>785882.92</v>
-      </c>
-      <c r="W5" s="25">
-        <v>754111.61</v>
-      </c>
-      <c r="X5" s="25">
-        <v>711427.81</v>
-      </c>
-      <c r="Y5" s="41">
-        <f>+(1-0.096)*X5</f>
-        <v>643130.74024000007</v>
-      </c>
-      <c r="Z5" s="41">
-        <f>+(1+0.045)*Y5</f>
-        <v>672071.62355080002</v>
+      <c r="B5">
+        <v>887993.35532922589</v>
+      </c>
+      <c r="C5">
+        <v>879036.18431822874</v>
+      </c>
+      <c r="D5">
+        <v>855915.47088362614</v>
+      </c>
+      <c r="E5">
+        <v>854428.31400453474</v>
+      </c>
+      <c r="F5">
+        <v>871672.55396098446</v>
+      </c>
+      <c r="G5">
+        <v>859047.3179795054</v>
+      </c>
+      <c r="H5">
+        <v>861991.41276048764</v>
+      </c>
+      <c r="I5">
+        <v>847525.76672442269</v>
+      </c>
+      <c r="J5">
+        <v>826317.63002991537</v>
+      </c>
+      <c r="K5">
+        <v>843777.14802887873</v>
+      </c>
+      <c r="L5">
+        <v>811068.20516096393</v>
+      </c>
+      <c r="M5">
+        <v>809368.41343896836</v>
+      </c>
+      <c r="N5">
+        <v>753589.85135223949</v>
+      </c>
+      <c r="O5">
+        <v>783163.26024122816</v>
+      </c>
+      <c r="P5">
+        <v>763689.91385910055</v>
+      </c>
+      <c r="Q5">
+        <v>773001.26369498728</v>
+      </c>
+      <c r="R5">
+        <v>797571.54298270063</v>
+      </c>
+      <c r="S5">
+        <v>751080.8174345498</v>
+      </c>
+      <c r="T5">
+        <v>755630.99826963618</v>
+      </c>
+      <c r="U5">
+        <v>770457.17858047294</v>
+      </c>
+      <c r="V5">
+        <v>760948.65197173611</v>
+      </c>
+      <c r="W5">
+        <v>733112.18503952282</v>
+      </c>
+      <c r="X5">
+        <v>680076.04134311411</v>
+      </c>
+      <c r="Y5">
+        <v>600785.00061489956</v>
+      </c>
+      <c r="Z5">
+        <v>628894.9879933527</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="33">
-        <v>267420.09000000003</v>
-      </c>
-      <c r="C6" s="33">
-        <v>276064.76</v>
-      </c>
-      <c r="D6" s="33">
-        <v>299540.27</v>
-      </c>
-      <c r="E6" s="33">
-        <v>311384.59000000003</v>
-      </c>
-      <c r="F6" s="33">
-        <v>313343.95</v>
-      </c>
-      <c r="G6" s="33">
-        <v>333447.05</v>
-      </c>
-      <c r="H6" s="33">
-        <v>337700.85</v>
-      </c>
-      <c r="I6" s="33">
-        <v>354611.85</v>
-      </c>
-      <c r="J6" s="33">
-        <v>369681.3</v>
-      </c>
-      <c r="K6" s="33">
-        <v>360702.6</v>
-      </c>
-      <c r="L6" s="33">
-        <v>368546.02</v>
-      </c>
-      <c r="M6" s="33">
-        <v>336767.46</v>
-      </c>
-      <c r="N6" s="33">
-        <v>297385.07</v>
-      </c>
-      <c r="O6" s="33">
-        <v>283872.71000000002</v>
-      </c>
-      <c r="P6" s="33">
-        <v>284729.53000000003</v>
-      </c>
-      <c r="Q6" s="33">
-        <v>278963.93</v>
-      </c>
-      <c r="R6" s="33">
-        <v>252726.12</v>
-      </c>
-      <c r="S6" s="33">
-        <v>255067.9</v>
-      </c>
-      <c r="T6" s="33">
-        <v>271694.2</v>
-      </c>
-      <c r="U6" s="33">
-        <v>260757.96</v>
-      </c>
-      <c r="V6" s="33">
-        <v>274641.96000000002</v>
-      </c>
-      <c r="W6" s="33">
-        <v>269713.44</v>
-      </c>
-      <c r="X6" s="33">
-        <v>251498.5</v>
-      </c>
-      <c r="Y6" s="41">
-        <f>+(1-0.189)*X6</f>
-        <v>203965.28349999999</v>
-      </c>
-      <c r="Z6" s="42">
-        <f>+(1+0.05)*Y6</f>
-        <v>214163.54767500001</v>
+      <c r="B6">
+        <v>263640.34135575831</v>
+      </c>
+      <c r="C6">
+        <v>274258.65299513598</v>
+      </c>
+      <c r="D6">
+        <v>298793.14028158406</v>
+      </c>
+      <c r="E6">
+        <v>309324.46122503962</v>
+      </c>
+      <c r="F6">
+        <v>313991.8503621681</v>
+      </c>
+      <c r="G6">
+        <v>332301.41009864205</v>
+      </c>
+      <c r="H6">
+        <v>340081.60005336895</v>
+      </c>
+      <c r="I6">
+        <v>362093.97793486062</v>
+      </c>
+      <c r="J6">
+        <v>374941.8566014244</v>
+      </c>
+      <c r="K6">
+        <v>369370.48219646729</v>
+      </c>
+      <c r="L6">
+        <v>380538.29693307856</v>
+      </c>
+      <c r="M6">
+        <v>354799.75480488141</v>
+      </c>
+      <c r="N6">
+        <v>316273.54260355624</v>
+      </c>
+      <c r="O6">
+        <v>300149.85692858341</v>
+      </c>
+      <c r="P6">
+        <v>308529.29223581881</v>
+      </c>
+      <c r="Q6">
+        <v>306274.06059806282</v>
+      </c>
+      <c r="R6">
+        <v>274507.7473573329</v>
+      </c>
+      <c r="S6">
+        <v>271854.03066250053</v>
+      </c>
+      <c r="T6">
+        <v>287870.17874594429</v>
+      </c>
+      <c r="U6">
+        <v>280621.32833896182</v>
+      </c>
+      <c r="V6">
+        <v>298251.51284009672</v>
+      </c>
+      <c r="W6">
+        <v>293007.69607476098</v>
+      </c>
+      <c r="X6">
+        <v>276158.84543109947</v>
+      </c>
+      <c r="Y6">
+        <v>223573.22731877086</v>
+      </c>
+      <c r="Z6">
+        <v>245722.95044553457</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -1238,79 +1197,79 @@
       <c r="A9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="42">
         <v>1997</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="42">
         <v>1998</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="42">
         <v>1999</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="42">
         <v>2000</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="42">
         <v>2001</v>
       </c>
-      <c r="G9" s="47">
+      <c r="G9" s="42">
         <v>2002</v>
       </c>
-      <c r="H9" s="47">
+      <c r="H9" s="42">
         <v>2003</v>
       </c>
-      <c r="I9" s="47">
+      <c r="I9" s="42">
         <v>2004</v>
       </c>
-      <c r="J9" s="47">
+      <c r="J9" s="42">
         <v>2005</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="42">
         <v>2006</v>
       </c>
-      <c r="L9" s="47">
+      <c r="L9" s="42">
         <v>2007</v>
       </c>
-      <c r="M9" s="47">
+      <c r="M9" s="42">
         <v>2008</v>
       </c>
-      <c r="N9" s="47">
+      <c r="N9" s="42">
         <v>2009</v>
       </c>
-      <c r="O9" s="47">
+      <c r="O9" s="42">
         <v>2010</v>
       </c>
-      <c r="P9" s="47">
+      <c r="P9" s="42">
         <v>2011</v>
       </c>
-      <c r="Q9" s="47">
+      <c r="Q9" s="42">
         <v>2012</v>
       </c>
-      <c r="R9" s="47">
+      <c r="R9" s="42">
         <v>2013</v>
       </c>
-      <c r="S9" s="47">
+      <c r="S9" s="42">
         <v>2014</v>
       </c>
-      <c r="T9" s="47">
+      <c r="T9" s="42">
         <v>2015</v>
       </c>
-      <c r="U9" s="47">
+      <c r="U9" s="42">
         <v>2016</v>
       </c>
-      <c r="V9" s="47">
+      <c r="V9" s="42">
         <v>2017</v>
       </c>
-      <c r="W9" s="48">
+      <c r="W9" s="43">
         <v>2018</v>
       </c>
-      <c r="X9" s="48">
+      <c r="X9" s="43">
         <v>2019</v>
       </c>
-      <c r="Y9" s="48">
+      <c r="Y9" s="43">
         <v>2020</v>
       </c>
-      <c r="Z9" s="34">
+      <c r="Z9" s="31">
         <v>2021</v>
       </c>
     </row>
@@ -1318,82 +1277,80 @@
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="33">
-        <v>325.36</v>
-      </c>
-      <c r="C10" s="33">
-        <v>322.56</v>
-      </c>
-      <c r="D10" s="33">
-        <v>315.57</v>
-      </c>
-      <c r="E10" s="33">
-        <v>317.13</v>
-      </c>
-      <c r="F10" s="33">
-        <v>327.12</v>
-      </c>
-      <c r="G10" s="33">
-        <v>319.41000000000003</v>
-      </c>
-      <c r="H10" s="33">
-        <v>321.92</v>
-      </c>
-      <c r="I10" s="33">
-        <v>323.70999999999998</v>
-      </c>
-      <c r="J10" s="33">
-        <v>321.62</v>
-      </c>
-      <c r="K10" s="33">
-        <v>332.75</v>
-      </c>
-      <c r="L10" s="33">
-        <v>315.79000000000002</v>
-      </c>
-      <c r="M10" s="33">
-        <v>320.76</v>
-      </c>
-      <c r="N10" s="33">
-        <v>299.92</v>
-      </c>
-      <c r="O10" s="33">
-        <v>315.14999999999998</v>
-      </c>
-      <c r="P10" s="36">
-        <v>297.8</v>
-      </c>
-      <c r="Q10" s="33">
-        <v>301.12</v>
-      </c>
-      <c r="R10" s="33">
-        <v>308.29000000000002</v>
-      </c>
-      <c r="S10" s="36">
-        <v>293.60000000000002</v>
-      </c>
-      <c r="T10" s="33">
-        <v>295.93</v>
-      </c>
-      <c r="U10" s="33">
-        <v>297.63</v>
-      </c>
-      <c r="V10" s="33">
-        <v>298.12</v>
-      </c>
-      <c r="W10" s="33">
-        <v>291.95</v>
-      </c>
-      <c r="X10" s="33">
-        <v>285.24</v>
-      </c>
-      <c r="Y10" s="41">
-        <f>+(1-0.08)*X10</f>
-        <v>262.42080000000004</v>
-      </c>
-      <c r="Z10" s="41">
-        <f>+(1+0.026)*Y10</f>
-        <v>269.24374080000007</v>
+      <c r="B10" s="30">
+        <v>348511.36098922254</v>
+      </c>
+      <c r="C10" s="30">
+        <v>345626.10964036058</v>
+      </c>
+      <c r="D10" s="30">
+        <v>340804.84562929464</v>
+      </c>
+      <c r="E10" s="30">
+        <v>342921.68612607627</v>
+      </c>
+      <c r="F10" s="30">
+        <v>349337.85486954253</v>
+      </c>
+      <c r="G10" s="30">
+        <v>344946.08243607194</v>
+      </c>
+      <c r="H10" s="30">
+        <v>344838.43103842839</v>
+      </c>
+      <c r="I10" s="30">
+        <v>344788.7535117878</v>
+      </c>
+      <c r="J10" s="30">
+        <v>340724.96475210856</v>
+      </c>
+      <c r="K10" s="30">
+        <v>349302.18287823233</v>
+      </c>
+      <c r="L10" s="30">
+        <v>334774.26623061975</v>
+      </c>
+      <c r="M10" s="30">
+        <v>338319.97166514868</v>
+      </c>
+      <c r="N10" s="30">
+        <v>317470.3534185976</v>
+      </c>
+      <c r="O10" s="30">
+        <v>330795.37306064123</v>
+      </c>
+      <c r="P10" s="33">
+        <v>319052.99421121448</v>
+      </c>
+      <c r="Q10" s="30">
+        <v>323466.44493911543</v>
+      </c>
+      <c r="R10" s="30">
+        <v>332632.791522933</v>
+      </c>
+      <c r="S10" s="33">
+        <v>318834.90754421824</v>
+      </c>
+      <c r="T10" s="30">
+        <v>324885.7406898663</v>
+      </c>
+      <c r="U10" s="30">
+        <v>330224.57503649796</v>
+      </c>
+      <c r="V10" s="30">
+        <v>334511.03916733386</v>
+      </c>
+      <c r="W10" s="30">
+        <v>326126.35813035053</v>
+      </c>
+      <c r="X10" s="30">
+        <v>317730.1670567696</v>
+      </c>
+      <c r="Y10" s="38">
+        <v>295130.91271534777</v>
+      </c>
+      <c r="Z10" s="38">
+        <v>301942.14680676471</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1401,108 +1358,106 @@
         <v>1</v>
       </c>
       <c r="B11" s="25">
-        <v>99.54</v>
+        <v>114913.5907023129</v>
       </c>
       <c r="C11" s="25">
-        <v>103.87</v>
+        <v>120454.19029669376</v>
       </c>
       <c r="D11" s="25">
-        <v>109.73</v>
+        <v>124136.18072154273</v>
       </c>
       <c r="E11" s="25">
-        <v>114.53</v>
+        <v>131353.13734318217</v>
       </c>
       <c r="F11" s="25">
-        <v>117.54</v>
-      </c>
-      <c r="G11" s="37">
-        <v>121.3</v>
+        <v>137390.63740147848</v>
+      </c>
+      <c r="G11" s="34">
+        <v>138871.45782041483</v>
       </c>
       <c r="H11" s="25">
-        <v>126.05</v>
+        <v>146764.36851586634</v>
       </c>
       <c r="I11" s="25">
-        <v>132.82</v>
+        <v>152134.98008836794</v>
       </c>
       <c r="J11" s="25">
-        <v>136.03</v>
+        <v>153176.88490017841</v>
       </c>
       <c r="K11" s="25">
-        <v>136.21</v>
+        <v>155391.22866454997</v>
       </c>
       <c r="L11" s="25">
-        <v>138.84</v>
+        <v>158798.49242442884</v>
       </c>
       <c r="M11" s="25">
-        <v>133.91999999999999</v>
+        <v>154412.29531194485</v>
       </c>
       <c r="N11" s="25">
-        <v>123.02</v>
+        <v>143147.54549532515</v>
       </c>
       <c r="O11" s="25">
-        <v>123.01</v>
+        <v>147023.41429572518</v>
       </c>
       <c r="P11" s="25">
-        <v>122.68</v>
+        <v>144250.16341427216</v>
       </c>
       <c r="Q11" s="25">
-        <v>123.05</v>
+        <v>143450.21457585317</v>
       </c>
       <c r="R11" s="25">
-        <v>115.69</v>
+        <v>136276.09005545735</v>
       </c>
       <c r="S11" s="25">
-        <v>113.84</v>
+        <v>133753.32544449164</v>
       </c>
       <c r="T11" s="25">
-        <v>118.18</v>
+        <v>135422.37657955798</v>
       </c>
       <c r="U11" s="25">
-        <v>118.46</v>
+        <v>136713.17766634878</v>
       </c>
       <c r="V11" s="25">
-        <v>124.94</v>
+        <v>138272.65802599379</v>
       </c>
       <c r="W11" s="25">
-        <v>124.33</v>
+        <v>140763.56309210692</v>
       </c>
       <c r="X11" s="25">
-        <v>120.66</v>
-      </c>
-      <c r="Y11" s="41">
-        <f>+(1-0.114)*X11</f>
-        <v>106.90476</v>
-      </c>
-      <c r="Z11" s="42">
-        <f>+(1+0.05)*Y11</f>
-        <v>112.24999800000001</v>
+        <v>136834.42513753468</v>
+      </c>
+      <c r="Y11" s="38">
+        <v>123770.1790531929</v>
+      </c>
+      <c r="Z11" s="39">
+        <v>133553.79230005638</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
-      <c r="V12" s="46"/>
-      <c r="W12" s="46"/>
-      <c r="X12" s="46"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="45"/>
     </row>
     <row r="13" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
@@ -1516,79 +1471,79 @@
       <c r="A14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="42">
         <v>1997</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="42">
         <v>1998</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="42">
         <v>1999</v>
       </c>
-      <c r="E14" s="47">
+      <c r="E14" s="42">
         <v>2000</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="42">
         <v>2001</v>
       </c>
-      <c r="G14" s="47">
+      <c r="G14" s="42">
         <v>2002</v>
       </c>
-      <c r="H14" s="47">
+      <c r="H14" s="42">
         <v>2003</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="42">
         <v>2004</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="42">
         <v>2005</v>
       </c>
-      <c r="K14" s="47">
+      <c r="K14" s="42">
         <v>2006</v>
       </c>
-      <c r="L14" s="47">
+      <c r="L14" s="42">
         <v>2007</v>
       </c>
-      <c r="M14" s="47">
+      <c r="M14" s="42">
         <v>2008</v>
       </c>
-      <c r="N14" s="47">
+      <c r="N14" s="42">
         <v>2009</v>
       </c>
-      <c r="O14" s="47">
+      <c r="O14" s="42">
         <v>2010</v>
       </c>
-      <c r="P14" s="47">
+      <c r="P14" s="42">
         <v>2011</v>
       </c>
-      <c r="Q14" s="47">
+      <c r="Q14" s="42">
         <v>2012</v>
       </c>
-      <c r="R14" s="47">
+      <c r="R14" s="42">
         <v>2013</v>
       </c>
-      <c r="S14" s="47">
+      <c r="S14" s="42">
         <v>2014</v>
       </c>
-      <c r="T14" s="47">
+      <c r="T14" s="42">
         <v>2015</v>
       </c>
-      <c r="U14" s="47">
+      <c r="U14" s="42">
         <v>2016</v>
       </c>
-      <c r="V14" s="47">
+      <c r="V14" s="42">
         <v>2017</v>
       </c>
-      <c r="W14" s="48">
+      <c r="W14" s="43">
         <v>2018</v>
       </c>
-      <c r="X14" s="48">
+      <c r="X14" s="43">
         <v>2019</v>
       </c>
-      <c r="Y14" s="48">
+      <c r="Y14" s="43">
         <v>2020</v>
       </c>
-      <c r="Z14" s="34">
+      <c r="Z14" s="31">
         <v>2021</v>
       </c>
     </row>
@@ -1596,73 +1551,73 @@
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="30">
         <v>2389169.1</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="30">
         <v>2437285.4</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="30">
         <v>2483283.2999999998</v>
       </c>
       <c r="E15" s="27">
         <v>2555609</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="30">
         <v>2598580.7999999998</v>
       </c>
-      <c r="G15" s="33">
+      <c r="G15" s="30">
         <v>2593436.2999999998</v>
       </c>
-      <c r="H15" s="33">
+      <c r="H15" s="30">
         <v>2575279.2000000002</v>
       </c>
       <c r="I15" s="27">
         <v>2605541</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="30">
         <v>2624605.9</v>
       </c>
-      <c r="K15" s="33">
+      <c r="K15" s="30">
         <v>2724772.5</v>
       </c>
-      <c r="L15" s="33">
+      <c r="L15" s="30">
         <v>2805874.1</v>
       </c>
-      <c r="M15" s="33">
+      <c r="M15" s="30">
         <v>2832807.1</v>
       </c>
-      <c r="N15" s="33">
+      <c r="N15" s="30">
         <v>2671511.7000000002</v>
       </c>
-      <c r="O15" s="33">
+      <c r="O15" s="30">
         <v>2783177.8</v>
       </c>
-      <c r="P15" s="33">
+      <c r="P15" s="30">
         <v>2892422.8</v>
       </c>
-      <c r="Q15" s="33">
+      <c r="Q15" s="30">
         <v>2904527.6</v>
       </c>
-      <c r="R15" s="33">
+      <c r="R15" s="30">
         <v>2917237.5</v>
       </c>
-      <c r="S15" s="33">
+      <c r="S15" s="30">
         <v>2981695.2</v>
       </c>
       <c r="T15" s="27">
         <v>3026180</v>
       </c>
-      <c r="U15" s="33">
+      <c r="U15" s="30">
         <v>3093663.8</v>
       </c>
-      <c r="V15" s="33">
+      <c r="V15" s="30">
         <v>3176581.2</v>
       </c>
-      <c r="W15" s="33">
+      <c r="W15" s="30">
         <v>3211079.6</v>
       </c>
-      <c r="X15" s="33">
+      <c r="X15" s="30">
         <v>3244972.8</v>
       </c>
       <c r="Y15" s="27">
@@ -1671,7 +1626,7 @@
       <c r="Z15" s="27">
         <v>3186264.9</v>
       </c>
-      <c r="AB15" s="35"/>
+      <c r="AB15" s="32"/>
     </row>
     <row r="16" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1750,106 +1705,34 @@
         <v>1064616</v>
       </c>
       <c r="Z16" s="26">
-        <v>1117424</v>
+        <v>1119225</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C17" s="35">
-        <f>+(C16-B16)/B16</f>
-        <v>4.3930373512449321E-2</v>
-      </c>
-      <c r="D17" s="35">
-        <f t="shared" ref="D17:Y17" si="0">+(D16-C16)/C16</f>
-        <v>4.4904913155355421E-2</v>
-      </c>
-      <c r="E17" s="35">
-        <f t="shared" si="0"/>
-        <v>5.2459946804161398E-2</v>
-      </c>
-      <c r="F17" s="35">
-        <f t="shared" si="0"/>
-        <v>3.9329488433309877E-2</v>
-      </c>
-      <c r="G17" s="35">
-        <f t="shared" si="0"/>
-        <v>2.7310222316026454E-2</v>
-      </c>
-      <c r="H17" s="35">
-        <f t="shared" si="0"/>
-        <v>2.9818948359620776E-2</v>
-      </c>
-      <c r="I17" s="35">
-        <f t="shared" si="0"/>
-        <v>3.1227952415142451E-2</v>
-      </c>
-      <c r="J17" s="35">
-        <f t="shared" si="0"/>
-        <v>3.6520326743317871E-2</v>
-      </c>
-      <c r="K17" s="35">
-        <f t="shared" si="0"/>
-        <v>4.102727115424621E-2</v>
-      </c>
-      <c r="L17" s="35">
-        <f t="shared" si="0"/>
-        <v>3.6046879712693214E-2</v>
-      </c>
-      <c r="M17" s="35">
-        <f t="shared" si="0"/>
-        <v>8.8714518248530442E-3</v>
-      </c>
-      <c r="N17" s="35">
-        <f t="shared" si="0"/>
-        <v>-3.7632319269008903E-2</v>
-      </c>
-      <c r="O17" s="35">
-        <f t="shared" si="0"/>
-        <v>1.6301023084142427E-3</v>
-      </c>
-      <c r="P17" s="35">
-        <f t="shared" si="0"/>
-        <v>-8.1437345515107205E-3</v>
-      </c>
-      <c r="Q17" s="35">
-        <f t="shared" si="0"/>
-        <v>-2.9594413017355603E-2</v>
-      </c>
-      <c r="R17" s="35">
-        <f t="shared" si="0"/>
-        <v>-1.4353942591932829E-2</v>
-      </c>
-      <c r="S17" s="35">
-        <f t="shared" si="0"/>
-        <v>1.3839079426702995E-2</v>
-      </c>
-      <c r="T17" s="35">
-        <f t="shared" si="0"/>
-        <v>3.8351726603384699E-2</v>
-      </c>
-      <c r="U17" s="35">
-        <f t="shared" si="0"/>
-        <v>3.0313013298193189E-2</v>
-      </c>
-      <c r="V17" s="35">
-        <f t="shared" si="0"/>
-        <v>2.973641190537309E-2</v>
-      </c>
-      <c r="W17" s="35">
-        <f t="shared" si="0"/>
-        <v>2.2887856761744818E-2</v>
-      </c>
-      <c r="X17" s="35">
-        <f t="shared" si="0"/>
-        <v>2.0851914211710423E-2</v>
-      </c>
-      <c r="Y17" s="35">
-        <f t="shared" si="0"/>
-        <v>-0.10822886493966437</v>
-      </c>
-      <c r="Z17" s="35">
-        <f>+(Z16-Y16)/Y16</f>
-        <v>4.9602861501236127E-2</v>
-      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="32"/>
     </row>
     <row r="18" spans="1:26" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
@@ -1860,240 +1743,240 @@
       <c r="A19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="42">
         <v>1997</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="42">
         <v>1998</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="42">
         <v>1999</v>
       </c>
-      <c r="E19" s="47">
+      <c r="E19" s="42">
         <v>2000</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F19" s="42">
         <v>2001</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="42">
         <v>2002</v>
       </c>
-      <c r="H19" s="47">
+      <c r="H19" s="42">
         <v>2003</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="42">
         <v>2004</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="42">
         <v>2005</v>
       </c>
-      <c r="K19" s="47">
+      <c r="K19" s="42">
         <v>2006</v>
       </c>
-      <c r="L19" s="47">
+      <c r="L19" s="42">
         <v>2007</v>
       </c>
-      <c r="M19" s="47">
+      <c r="M19" s="42">
         <v>2008</v>
       </c>
-      <c r="N19" s="47">
+      <c r="N19" s="42">
         <v>2009</v>
       </c>
-      <c r="O19" s="47">
+      <c r="O19" s="42">
         <v>2010</v>
       </c>
-      <c r="P19" s="47">
+      <c r="P19" s="42">
         <v>2011</v>
       </c>
-      <c r="Q19" s="47">
+      <c r="Q19" s="42">
         <v>2012</v>
       </c>
-      <c r="R19" s="47">
+      <c r="R19" s="42">
         <v>2013</v>
       </c>
-      <c r="S19" s="47">
+      <c r="S19" s="42">
         <v>2014</v>
       </c>
-      <c r="T19" s="47">
+      <c r="T19" s="42">
         <v>2015</v>
       </c>
-      <c r="U19" s="47">
+      <c r="U19" s="42">
         <v>2016</v>
       </c>
-      <c r="V19" s="47">
+      <c r="V19" s="42">
         <v>2017</v>
       </c>
-      <c r="W19" s="48">
+      <c r="W19" s="43">
         <v>2018</v>
       </c>
-      <c r="X19" s="48">
+      <c r="X19" s="43">
         <v>2019</v>
       </c>
-      <c r="Y19" s="48">
+      <c r="Y19" s="43">
         <v>2020</v>
       </c>
-      <c r="Z19" s="34">
+      <c r="Z19" s="31">
         <v>2021</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="39">
-        <v>82012162</v>
-      </c>
-      <c r="C20" s="39">
+      <c r="B20" s="36">
         <v>82057379</v>
       </c>
-      <c r="D20" s="39">
+      <c r="C20" s="36">
         <v>82037011</v>
       </c>
-      <c r="E20" s="39">
+      <c r="D20" s="36">
         <v>82163475</v>
       </c>
-      <c r="F20" s="39">
+      <c r="E20" s="36">
         <v>82259540</v>
       </c>
-      <c r="G20" s="39">
+      <c r="F20" s="36">
         <v>82440309</v>
       </c>
-      <c r="H20" s="39">
+      <c r="G20" s="36">
         <v>82536680</v>
       </c>
-      <c r="I20" s="39">
+      <c r="H20" s="36">
         <v>82531671</v>
       </c>
-      <c r="J20" s="39">
+      <c r="I20" s="36">
         <v>82500849</v>
       </c>
-      <c r="K20" s="39">
+      <c r="J20" s="36">
         <v>82437995</v>
       </c>
-      <c r="L20" s="39">
+      <c r="K20" s="36">
         <v>82314906</v>
       </c>
-      <c r="M20" s="39">
+      <c r="L20" s="36">
         <v>82217837</v>
       </c>
-      <c r="N20" s="39">
+      <c r="M20" s="36">
         <v>82002356</v>
       </c>
-      <c r="O20" s="39">
+      <c r="N20" s="36">
         <v>81802257</v>
       </c>
-      <c r="P20" s="39">
+      <c r="O20" s="36">
         <v>80222065</v>
       </c>
-      <c r="Q20" s="39">
+      <c r="P20" s="36">
         <v>80327900</v>
       </c>
-      <c r="R20" s="39">
+      <c r="Q20" s="36">
         <v>80523746</v>
       </c>
-      <c r="S20" s="39">
+      <c r="R20" s="36">
         <v>80767463</v>
       </c>
-      <c r="T20" s="39">
+      <c r="S20" s="36">
         <v>81197537</v>
       </c>
-      <c r="U20" s="39">
+      <c r="T20" s="36">
         <v>82175684</v>
       </c>
-      <c r="V20" s="39">
+      <c r="U20" s="36">
         <v>82521653</v>
       </c>
-      <c r="W20" s="39">
+      <c r="V20" s="36">
         <v>82792351</v>
       </c>
-      <c r="X20" s="39">
+      <c r="W20" s="36">
         <v>83019213</v>
       </c>
-      <c r="Y20" s="39">
+      <c r="X20" s="36">
         <v>83166711</v>
       </c>
-      <c r="Z20" s="39">
+      <c r="Y20" s="36">
         <v>83155031</v>
       </c>
+      <c r="Z20" s="36">
+        <v>83237124</v>
+      </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="40">
-        <v>40049974</v>
-      </c>
-      <c r="C21" s="40">
-        <v>40214066</v>
-      </c>
-      <c r="D21" s="40">
-        <v>40369667</v>
-      </c>
-      <c r="E21" s="40">
-        <v>40554387</v>
-      </c>
-      <c r="F21" s="40">
-        <v>40766049</v>
-      </c>
-      <c r="G21" s="40">
-        <v>41423520</v>
-      </c>
-      <c r="H21" s="40">
-        <v>42196231</v>
-      </c>
-      <c r="I21" s="40">
-        <v>42859172</v>
-      </c>
-      <c r="J21" s="40">
-        <v>43662613</v>
-      </c>
-      <c r="K21" s="40">
-        <v>44360521</v>
-      </c>
-      <c r="L21" s="40">
-        <v>45236004</v>
-      </c>
-      <c r="M21" s="40">
-        <v>45983169</v>
-      </c>
-      <c r="N21" s="40">
-        <v>46367550</v>
-      </c>
-      <c r="O21" s="40">
-        <v>46562483</v>
-      </c>
-      <c r="P21" s="40">
-        <v>46736257</v>
-      </c>
-      <c r="Q21" s="40">
-        <v>46766403</v>
-      </c>
-      <c r="R21" s="40">
-        <v>46593236</v>
-      </c>
-      <c r="S21" s="40">
-        <v>46455123</v>
-      </c>
-      <c r="T21" s="40">
-        <v>46410149</v>
-      </c>
-      <c r="U21" s="40">
-        <v>46449874</v>
-      </c>
-      <c r="V21" s="40">
-        <v>46532869</v>
-      </c>
-      <c r="W21" s="40">
-        <v>46728814</v>
-      </c>
-      <c r="X21" s="40">
-        <v>47105358</v>
-      </c>
-      <c r="Y21" s="40">
-        <v>47355685</v>
-      </c>
-      <c r="Z21" s="40">
-        <v>47326687</v>
+      <c r="B21" s="37">
+        <v>40143449</v>
+      </c>
+      <c r="C21" s="37">
+        <v>40303568</v>
+      </c>
+      <c r="D21" s="37">
+        <v>40470182</v>
+      </c>
+      <c r="E21" s="37">
+        <v>40665545</v>
+      </c>
+      <c r="F21" s="37">
+        <v>41035278</v>
+      </c>
+      <c r="G21" s="37">
+        <v>41827838</v>
+      </c>
+      <c r="H21" s="37">
+        <v>42547451</v>
+      </c>
+      <c r="I21" s="37">
+        <v>43296338</v>
+      </c>
+      <c r="J21" s="37">
+        <v>44009971</v>
+      </c>
+      <c r="K21" s="37">
+        <v>44784666</v>
+      </c>
+      <c r="L21" s="37">
+        <v>45668939</v>
+      </c>
+      <c r="M21" s="37">
+        <v>46239273</v>
+      </c>
+      <c r="N21" s="37">
+        <v>46486619</v>
+      </c>
+      <c r="O21" s="37">
+        <v>46667174</v>
+      </c>
+      <c r="P21" s="37">
+        <v>46818219</v>
+      </c>
+      <c r="Q21" s="37">
+        <v>46727890</v>
+      </c>
+      <c r="R21" s="37">
+        <v>46512199</v>
+      </c>
+      <c r="S21" s="37">
+        <v>46449565</v>
+      </c>
+      <c r="T21" s="37">
+        <v>46440099</v>
+      </c>
+      <c r="U21" s="37">
+        <v>46528024</v>
+      </c>
+      <c r="V21" s="37">
+        <v>46658447</v>
+      </c>
+      <c r="W21" s="37">
+        <v>46937060</v>
+      </c>
+      <c r="X21" s="37">
+        <v>47332614</v>
+      </c>
+      <c r="Y21" s="37">
+        <v>47398695</v>
+      </c>
+      <c r="Z21" s="37">
+        <v>47432805</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
@@ -2110,79 +1993,79 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="39">
+      <c r="B24" s="36">
         <v>39971329</v>
       </c>
-      <c r="C24" s="39">
+      <c r="C24" s="36">
         <v>40143449</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="36">
         <v>40303568</v>
       </c>
-      <c r="E24" s="39">
+      <c r="E24" s="36">
         <v>40470182</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="36">
         <v>40665545</v>
       </c>
-      <c r="G24" s="39">
+      <c r="G24" s="36">
         <v>41035278</v>
       </c>
-      <c r="H24" s="39">
+      <c r="H24" s="36">
         <v>41827838</v>
       </c>
-      <c r="I24" s="39">
+      <c r="I24" s="36">
         <v>42547451</v>
       </c>
-      <c r="J24" s="39">
+      <c r="J24" s="36">
         <v>43296338</v>
       </c>
-      <c r="K24" s="39">
+      <c r="K24" s="36">
         <v>44009971</v>
       </c>
-      <c r="L24" s="39">
+      <c r="L24" s="36">
         <v>44784666</v>
       </c>
-      <c r="M24" s="39">
+      <c r="M24" s="36">
         <v>45668939</v>
       </c>
-      <c r="N24" s="39">
+      <c r="N24" s="36">
         <v>46239273</v>
       </c>
-      <c r="O24" s="39">
+      <c r="O24" s="36">
         <v>46486619</v>
       </c>
-      <c r="P24" s="39">
+      <c r="P24" s="36">
         <v>46667174</v>
       </c>
-      <c r="Q24" s="39">
+      <c r="Q24" s="36">
         <v>46818219</v>
       </c>
-      <c r="R24" s="39">
+      <c r="R24" s="36">
         <v>46727890</v>
       </c>
-      <c r="S24" s="39">
+      <c r="S24" s="36">
         <v>46512199</v>
       </c>
-      <c r="T24" s="39">
+      <c r="T24" s="36">
         <v>46449565</v>
       </c>
-      <c r="U24" s="39">
+      <c r="U24" s="36">
         <v>46440099</v>
       </c>
-      <c r="V24" s="39">
+      <c r="V24" s="36">
         <v>46528024</v>
       </c>
-      <c r="W24" s="39">
+      <c r="W24" s="36">
         <v>46658447</v>
       </c>
-      <c r="X24" s="39">
+      <c r="X24" s="36">
         <v>46937060</v>
       </c>
-      <c r="Y24" s="39">
+      <c r="Y24" s="36">
         <v>47332614</v>
       </c>
-      <c r="Z24" s="39">
+      <c r="Z24" s="36">
         <v>47398695</v>
       </c>
     </row>
@@ -2201,14 +2084,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A833650B-A3F7-415B-A253-D92CCB3E5A53}">
   <dimension ref="A2:X20"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13:X20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
     <col min="22" max="23" width="9.83203125" bestFit="1" customWidth="1"/>
@@ -2218,7 +2101,7 @@
       <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="28" t="s">
@@ -2229,142 +2112,142 @@
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="42">
         <v>1997</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="42">
         <v>1998</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="42">
         <v>1999</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="42">
         <v>2000</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="42">
         <v>2001</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="42">
         <v>2002</v>
       </c>
-      <c r="H3" s="47">
+      <c r="H3" s="42">
         <v>2003</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="42">
         <v>2004</v>
       </c>
-      <c r="J3" s="47">
+      <c r="J3" s="42">
         <v>2005</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="42">
         <v>2006</v>
       </c>
-      <c r="L3" s="47">
+      <c r="L3" s="42">
         <v>2007</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="42">
         <v>2008</v>
       </c>
-      <c r="N3" s="47">
+      <c r="N3" s="42">
         <v>2009</v>
       </c>
-      <c r="O3" s="47">
+      <c r="O3" s="42">
         <v>2010</v>
       </c>
-      <c r="P3" s="47">
+      <c r="P3" s="42">
         <v>2011</v>
       </c>
-      <c r="Q3" s="47">
+      <c r="Q3" s="42">
         <v>2012</v>
       </c>
-      <c r="R3" s="47">
+      <c r="R3" s="42">
         <v>2013</v>
       </c>
-      <c r="S3" s="47">
+      <c r="S3" s="42">
         <v>2014</v>
       </c>
-      <c r="T3" s="47">
+      <c r="T3" s="42">
         <v>2015</v>
       </c>
-      <c r="U3" s="47">
+      <c r="U3" s="42">
         <v>2016</v>
       </c>
-      <c r="V3" s="47">
+      <c r="V3" s="42">
         <v>2017</v>
       </c>
-      <c r="W3" s="48">
+      <c r="W3" s="43">
         <v>2018</v>
       </c>
-      <c r="X3" s="34"/>
+      <c r="X3" s="31"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="46">
         <v>139421.04999999999</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="46">
         <v>135082.96</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="46">
         <v>132682.74</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="46">
         <v>129219.18</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="46">
         <v>122068.47</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="46">
         <v>121182.22</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="46">
         <v>117977.89</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="47">
         <v>117702</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="46">
         <v>114591.86</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="46">
         <v>119470.94</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="46">
         <v>127273.69</v>
       </c>
-      <c r="M4" s="31">
+      <c r="M4" s="46">
         <v>127417.96</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="46">
         <v>109326.74</v>
       </c>
-      <c r="O4" s="31">
+      <c r="O4" s="46">
         <v>124748.9</v>
       </c>
-      <c r="P4" s="31">
+      <c r="P4" s="46">
         <v>121825.78</v>
       </c>
-      <c r="Q4" s="31">
+      <c r="Q4" s="46">
         <v>116975.73</v>
       </c>
-      <c r="R4" s="31">
+      <c r="R4" s="46">
         <v>117694.75</v>
       </c>
-      <c r="S4" s="29">
+      <c r="S4" s="47">
         <v>117500</v>
       </c>
-      <c r="T4" s="31">
+      <c r="T4" s="46">
         <v>126140.8</v>
       </c>
-      <c r="U4" s="31">
+      <c r="U4" s="46">
         <v>128479.24</v>
       </c>
-      <c r="V4" s="31">
+      <c r="V4" s="46">
         <v>130422.76</v>
       </c>
-      <c r="W4" s="31">
+      <c r="W4" s="46">
         <v>125290.33</v>
       </c>
       <c r="X4" s="9"/>
@@ -2373,70 +2256,70 @@
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="48">
         <v>53125.87</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="48">
         <v>53062.92</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="48">
         <v>54795.45</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="48">
         <v>57874.34</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="48">
         <v>60180.66</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="48">
         <v>62823.72</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="48">
         <v>67381.27</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="48">
         <v>67407.66</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="48">
         <v>68396.44</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="48">
         <v>58441.74</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="48">
         <v>60386.35</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="48">
         <v>56928.68</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="48">
         <v>47107.43</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="48">
         <v>48813.83</v>
       </c>
-      <c r="P5" s="30">
+      <c r="P5" s="48">
         <v>45648.5</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="Q5" s="48">
         <v>44392.29</v>
       </c>
-      <c r="R5" s="30">
+      <c r="R5" s="48">
         <v>41267.379999999997</v>
       </c>
-      <c r="S5" s="30">
+      <c r="S5" s="48">
         <v>38602.300000000003</v>
       </c>
-      <c r="T5" s="30">
+      <c r="T5" s="48">
         <v>39081.9</v>
       </c>
-      <c r="U5" s="30">
+      <c r="U5" s="48">
         <v>39499.68</v>
       </c>
-      <c r="V5" s="30">
+      <c r="V5" s="48">
         <v>43255.8</v>
       </c>
-      <c r="W5" s="30">
+      <c r="W5" s="48">
         <v>45257.67</v>
       </c>
       <c r="X5" s="11"/>
@@ -2482,73 +2365,73 @@
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="42">
         <v>1997</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="42">
         <v>1998</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="42">
         <v>1999</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="42">
         <v>2000</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="42">
         <v>2001</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="42">
         <v>2002</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="42">
         <v>2003</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="42">
         <v>2004</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="42">
         <v>2005</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="42">
         <v>2006</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="42">
         <v>2007</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="42">
         <v>2008</v>
       </c>
-      <c r="N8" s="47">
+      <c r="N8" s="42">
         <v>2009</v>
       </c>
-      <c r="O8" s="47">
+      <c r="O8" s="42">
         <v>2010</v>
       </c>
-      <c r="P8" s="47">
+      <c r="P8" s="42">
         <v>2011</v>
       </c>
-      <c r="Q8" s="47">
+      <c r="Q8" s="42">
         <v>2012</v>
       </c>
-      <c r="R8" s="47">
+      <c r="R8" s="42">
         <v>2013</v>
       </c>
-      <c r="S8" s="47">
+      <c r="S8" s="42">
         <v>2014</v>
       </c>
-      <c r="T8" s="47">
+      <c r="T8" s="42">
         <v>2015</v>
       </c>
-      <c r="U8" s="47">
+      <c r="U8" s="42">
         <v>2016</v>
       </c>
-      <c r="V8" s="47">
+      <c r="V8" s="42">
         <v>2017</v>
       </c>
-      <c r="W8" s="47">
+      <c r="W8" s="42">
         <v>2018</v>
       </c>
-      <c r="X8" s="45"/>
+      <c r="X8" s="41"/>
     </row>
     <row r="9" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2695,30 +2578,30 @@
       <c r="X10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="46"/>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
     </row>
     <row r="12" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
@@ -2735,73 +2618,73 @@
       <c r="A13" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="42">
         <v>1997</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="42">
         <v>1998</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="42">
         <v>1999</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="42">
         <v>2000</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="42">
         <v>2001</v>
       </c>
-      <c r="G13" s="47">
+      <c r="G13" s="42">
         <v>2002</v>
       </c>
-      <c r="H13" s="47">
+      <c r="H13" s="42">
         <v>2003</v>
       </c>
-      <c r="I13" s="47">
+      <c r="I13" s="42">
         <v>2004</v>
       </c>
-      <c r="J13" s="47">
+      <c r="J13" s="42">
         <v>2005</v>
       </c>
-      <c r="K13" s="47">
+      <c r="K13" s="42">
         <v>2006</v>
       </c>
-      <c r="L13" s="47">
+      <c r="L13" s="42">
         <v>2007</v>
       </c>
-      <c r="M13" s="47">
+      <c r="M13" s="42">
         <v>2008</v>
       </c>
-      <c r="N13" s="47">
+      <c r="N13" s="42">
         <v>2009</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="42">
         <v>2010</v>
       </c>
-      <c r="P13" s="47">
+      <c r="P13" s="42">
         <v>2011</v>
       </c>
-      <c r="Q13" s="47">
+      <c r="Q13" s="42">
         <v>2012</v>
       </c>
-      <c r="R13" s="47">
+      <c r="R13" s="42">
         <v>2013</v>
       </c>
-      <c r="S13" s="47">
+      <c r="S13" s="42">
         <v>2014</v>
       </c>
-      <c r="T13" s="47">
+      <c r="T13" s="42">
         <v>2015</v>
       </c>
-      <c r="U13" s="47">
+      <c r="U13" s="42">
         <v>2016</v>
       </c>
-      <c r="V13" s="47">
+      <c r="V13" s="42">
         <v>2017</v>
       </c>
-      <c r="W13" s="47">
+      <c r="W13" s="42">
         <v>2018</v>
       </c>
-      <c r="X13" s="45"/>
+      <c r="X13" s="41"/>
     </row>
     <row r="14" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2812,7 +2695,7 @@
         <v>600981.19999999995</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" ref="C14:W14" si="0">+C17+C19</f>
+        <f t="shared" ref="C14:W15" si="0">+C17+C19</f>
         <v>600602.19999999995</v>
       </c>
       <c r="D14" s="3">
@@ -2906,87 +2789,87 @@
         <v>181505</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" ref="C15:W15" si="1">+C18+C20</f>
+        <f t="shared" si="0"/>
         <v>190871</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>201637</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>212042</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>222093</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>225161</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>229257</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>230754</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>236318</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>242511</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>244937</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>240155</v>
       </c>
       <c r="N15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>215974</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>201706</v>
       </c>
       <c r="P15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>189248</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>175658</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>168272</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>169942</v>
       </c>
       <c r="T15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>178212</v>
       </c>
       <c r="U15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>183258</v>
       </c>
       <c r="V15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>191465</v>
       </c>
       <c r="W15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>191326</v>
       </c>
       <c r="X15" s="6"/>
@@ -3137,70 +3020,70 @@
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="8">
         <v>156645.9</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="8">
         <v>151587.1</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="8">
         <v>150400.5</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="8">
         <v>147290.29999999999</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="8">
         <v>138197.1</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="18">
         <v>132289</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="8">
         <v>126218.5</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="8">
         <v>122433.8</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="8">
         <v>117400.1</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="8">
         <v>117337.60000000001</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="8">
         <v>116450.8</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="8">
         <v>115813.8</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="8">
         <v>112091.5</v>
       </c>
-      <c r="O19" s="25">
+      <c r="O19" s="8">
         <v>120672.7</v>
       </c>
-      <c r="P19" s="26">
+      <c r="P19" s="18">
         <v>124857</v>
       </c>
-      <c r="Q19" s="25">
+      <c r="Q19" s="8">
         <v>123308.2</v>
       </c>
-      <c r="R19" s="25">
+      <c r="R19" s="8">
         <v>120260.5</v>
       </c>
-      <c r="S19" s="25">
+      <c r="S19" s="8">
         <v>125069.4</v>
       </c>
-      <c r="T19" s="26">
+      <c r="T19" s="18">
         <v>124907</v>
       </c>
-      <c r="U19" s="25">
+      <c r="U19" s="8">
         <v>127267.7</v>
       </c>
-      <c r="V19" s="25">
+      <c r="V19" s="8">
         <v>127242.8</v>
       </c>
-      <c r="W19" s="25">
+      <c r="W19" s="8">
         <v>129603.5</v>
       </c>
     </row>
@@ -3208,70 +3091,70 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="19">
         <v>69350</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="19">
         <v>72586</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="19">
         <v>77095</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="19">
         <v>81238</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="19">
         <v>86820</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="19">
         <v>89703</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20" s="19">
         <v>91788</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="19">
         <v>92735</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J20" s="19">
         <v>96432</v>
       </c>
-      <c r="K20" s="27">
+      <c r="K20" s="19">
         <v>99316</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="19">
         <v>100296</v>
       </c>
-      <c r="M20" s="27">
+      <c r="M20" s="19">
         <v>99224</v>
       </c>
-      <c r="N20" s="27">
+      <c r="N20" s="19">
         <v>91166</v>
       </c>
-      <c r="O20" s="27">
+      <c r="O20" s="19">
         <v>77334</v>
       </c>
-      <c r="P20" s="27">
+      <c r="P20" s="19">
         <v>66869</v>
       </c>
-      <c r="Q20" s="27">
+      <c r="Q20" s="19">
         <v>60436</v>
       </c>
-      <c r="R20" s="27">
+      <c r="R20" s="19">
         <v>54225</v>
       </c>
-      <c r="S20" s="27">
+      <c r="S20" s="19">
         <v>53534</v>
       </c>
-      <c r="T20" s="27">
+      <c r="T20" s="19">
         <v>56440</v>
       </c>
-      <c r="U20" s="27">
+      <c r="U20" s="19">
         <v>58649</v>
       </c>
-      <c r="V20" s="27">
+      <c r="V20" s="19">
         <v>59795</v>
       </c>
-      <c r="W20" s="27">
+      <c r="W20" s="19">
         <v>61167</v>
       </c>
     </row>
@@ -3288,8 +3171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435F6862-B05E-491A-9D37-A7AD01486670}">
   <dimension ref="A2:X15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W13" activeCellId="1" sqref="W8:X8 W13:X13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3301,10 +3184,10 @@
       <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="29" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3312,73 +3195,73 @@
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="42">
         <v>1997</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="42">
         <v>1998</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="42">
         <v>1999</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="42">
         <v>2000</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="42">
         <v>2001</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="42">
         <v>2002</v>
       </c>
-      <c r="H3" s="47">
+      <c r="H3" s="42">
         <v>2003</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="42">
         <v>2004</v>
       </c>
-      <c r="J3" s="47">
+      <c r="J3" s="42">
         <v>2005</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="42">
         <v>2006</v>
       </c>
-      <c r="L3" s="47">
+      <c r="L3" s="42">
         <v>2007</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="42">
         <v>2008</v>
       </c>
-      <c r="N3" s="47">
+      <c r="N3" s="42">
         <v>2009</v>
       </c>
-      <c r="O3" s="47">
+      <c r="O3" s="42">
         <v>2010</v>
       </c>
-      <c r="P3" s="47">
+      <c r="P3" s="42">
         <v>2011</v>
       </c>
-      <c r="Q3" s="47">
+      <c r="Q3" s="42">
         <v>2012</v>
       </c>
-      <c r="R3" s="47">
+      <c r="R3" s="42">
         <v>2013</v>
       </c>
-      <c r="S3" s="47">
+      <c r="S3" s="42">
         <v>2014</v>
       </c>
-      <c r="T3" s="47">
+      <c r="T3" s="42">
         <v>2015</v>
       </c>
-      <c r="U3" s="47">
+      <c r="U3" s="42">
         <v>2016</v>
       </c>
-      <c r="V3" s="47">
+      <c r="V3" s="42">
         <v>2017</v>
       </c>
-      <c r="W3" s="47">
+      <c r="W3" s="42">
         <v>2018</v>
       </c>
-      <c r="X3" s="45" t="s">
+      <c r="X3" s="41" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3386,70 +3269,70 @@
       <c r="A4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="8">
         <v>175624.08</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="8">
         <v>179137.34</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="8">
         <v>184374.27</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="8">
         <v>180604.01</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="8">
         <v>176877.63</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="8">
         <v>175025.77</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="8">
         <v>168701.17</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="8">
         <v>168236.45</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="8">
         <v>160314.19</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="8">
         <v>156588.04</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="8">
         <v>153416.57999999999</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="8">
         <v>153088.24</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="8">
         <v>152331.54</v>
       </c>
-      <c r="O4" s="25">
+      <c r="O4" s="8">
         <v>153039.70000000001</v>
       </c>
-      <c r="P4" s="25">
+      <c r="P4" s="8">
         <v>154881.81</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4" s="8">
         <v>153543.32</v>
       </c>
-      <c r="R4" s="25">
+      <c r="R4" s="8">
         <v>157891.37</v>
       </c>
-      <c r="S4" s="25">
+      <c r="S4" s="8">
         <v>158685.25</v>
       </c>
-      <c r="T4" s="25">
+      <c r="T4" s="8">
         <v>161235.32999999999</v>
       </c>
-      <c r="U4" s="25">
+      <c r="U4" s="8">
         <v>164390.84</v>
       </c>
-      <c r="V4" s="25">
+      <c r="V4" s="8">
         <v>167390.31</v>
       </c>
-      <c r="W4" s="25">
+      <c r="W4" s="8">
         <v>161950.76999999999</v>
       </c>
       <c r="X4" s="9" t="s">
@@ -3460,70 +3343,70 @@
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="10">
         <v>73122.289999999994</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="10">
         <v>79736.320000000007</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="10">
         <v>83429.929999999993</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="10">
         <v>85053.58</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="10">
         <v>89000.88</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="10">
         <v>90781.26</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="10">
         <v>95261.29</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="10">
         <v>98901.13</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="10">
         <v>101470.91</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="10">
         <v>104713.37</v>
       </c>
-      <c r="L5" s="33">
+      <c r="L5" s="10">
         <v>107020.95</v>
       </c>
-      <c r="M5" s="33">
+      <c r="M5" s="10">
         <v>101151.5</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="10">
         <v>93969.33</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5" s="10">
         <v>90652.32</v>
       </c>
-      <c r="P5" s="33">
+      <c r="P5" s="10">
         <v>85504.83</v>
       </c>
-      <c r="Q5" s="33">
+      <c r="Q5" s="10">
         <v>78405.8</v>
       </c>
-      <c r="R5" s="33">
+      <c r="R5" s="10">
         <v>79211.33</v>
       </c>
-      <c r="S5" s="33">
+      <c r="S5" s="10">
         <v>79483.649999999994</v>
       </c>
-      <c r="T5" s="33">
+      <c r="T5" s="10">
         <v>82561.490000000005</v>
       </c>
-      <c r="U5" s="33">
+      <c r="U5" s="10">
         <v>85372.57</v>
       </c>
-      <c r="V5" s="33">
+      <c r="V5" s="10">
         <v>88006.02</v>
       </c>
-      <c r="W5" s="33">
+      <c r="W5" s="10">
         <v>89209.32</v>
       </c>
       <c r="X5" s="11" t="s">
@@ -3563,7 +3446,7 @@
       <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="29" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3571,73 +3454,73 @@
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="42">
         <v>1997</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="42">
         <v>1998</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="42">
         <v>1999</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="42">
         <v>2000</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="42">
         <v>2001</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="42">
         <v>2002</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="42">
         <v>2003</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="42">
         <v>2004</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="42">
         <v>2005</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="42">
         <v>2006</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="42">
         <v>2007</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="42">
         <v>2008</v>
       </c>
-      <c r="N8" s="47">
+      <c r="N8" s="42">
         <v>2009</v>
       </c>
-      <c r="O8" s="47">
+      <c r="O8" s="42">
         <v>2010</v>
       </c>
-      <c r="P8" s="47">
+      <c r="P8" s="42">
         <v>2011</v>
       </c>
-      <c r="Q8" s="47">
+      <c r="Q8" s="42">
         <v>2012</v>
       </c>
-      <c r="R8" s="47">
+      <c r="R8" s="42">
         <v>2013</v>
       </c>
-      <c r="S8" s="47">
+      <c r="S8" s="42">
         <v>2014</v>
       </c>
-      <c r="T8" s="47">
+      <c r="T8" s="42">
         <v>2015</v>
       </c>
-      <c r="U8" s="47">
+      <c r="U8" s="42">
         <v>2016</v>
       </c>
-      <c r="V8" s="47">
+      <c r="V8" s="42">
         <v>2017</v>
       </c>
-      <c r="W8" s="47">
+      <c r="W8" s="42">
         <v>2018</v>
       </c>
-      <c r="X8" s="45" t="s">
+      <c r="X8" s="41" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3798,73 +3681,73 @@
       <c r="A13" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="42">
         <v>1997</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="42">
         <v>1998</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="42">
         <v>1999</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="42">
         <v>2000</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="42">
         <v>2001</v>
       </c>
-      <c r="G13" s="47">
+      <c r="G13" s="42">
         <v>2002</v>
       </c>
-      <c r="H13" s="47">
+      <c r="H13" s="42">
         <v>2003</v>
       </c>
-      <c r="I13" s="47">
+      <c r="I13" s="42">
         <v>2004</v>
       </c>
-      <c r="J13" s="47">
+      <c r="J13" s="42">
         <v>2005</v>
       </c>
-      <c r="K13" s="47">
+      <c r="K13" s="42">
         <v>2006</v>
       </c>
-      <c r="L13" s="47">
+      <c r="L13" s="42">
         <v>2007</v>
       </c>
-      <c r="M13" s="47">
+      <c r="M13" s="42">
         <v>2008</v>
       </c>
-      <c r="N13" s="47">
+      <c r="N13" s="42">
         <v>2009</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="42">
         <v>2010</v>
       </c>
-      <c r="P13" s="47">
+      <c r="P13" s="42">
         <v>2011</v>
       </c>
-      <c r="Q13" s="47">
+      <c r="Q13" s="42">
         <v>2012</v>
       </c>
-      <c r="R13" s="47">
+      <c r="R13" s="42">
         <v>2013</v>
       </c>
-      <c r="S13" s="47">
+      <c r="S13" s="42">
         <v>2014</v>
       </c>
-      <c r="T13" s="47">
+      <c r="T13" s="42">
         <v>2015</v>
       </c>
-      <c r="U13" s="47">
+      <c r="U13" s="42">
         <v>2016</v>
       </c>
-      <c r="V13" s="47">
+      <c r="V13" s="42">
         <v>2017</v>
       </c>
-      <c r="W13" s="47">
+      <c r="W13" s="42">
         <v>2018</v>
       </c>
-      <c r="X13" s="45" t="s">
+      <c r="X13" s="41" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4019,8 +3902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712A49B1-B69A-4BE2-A124-7AF0E08088AC}">
   <dimension ref="A2:Y15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X13" sqref="X13:Y13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4033,10 +3916,10 @@
       <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="40" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4044,76 +3927,76 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="42">
         <v>1997</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="42">
         <v>1998</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="42">
         <v>1999</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="42">
         <v>2000</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="42">
         <v>2001</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="42">
         <v>2002</v>
       </c>
-      <c r="H3" s="47">
+      <c r="H3" s="42">
         <v>2003</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="42">
         <v>2004</v>
       </c>
-      <c r="J3" s="47">
+      <c r="J3" s="42">
         <v>2005</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="42">
         <v>2006</v>
       </c>
-      <c r="L3" s="47">
+      <c r="L3" s="42">
         <v>2007</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="42">
         <v>2008</v>
       </c>
-      <c r="N3" s="47">
+      <c r="N3" s="42">
         <v>2009</v>
       </c>
-      <c r="O3" s="47">
+      <c r="O3" s="42">
         <v>2010</v>
       </c>
-      <c r="P3" s="47">
+      <c r="P3" s="42">
         <v>2011</v>
       </c>
-      <c r="Q3" s="47">
+      <c r="Q3" s="42">
         <v>2012</v>
       </c>
-      <c r="R3" s="47">
+      <c r="R3" s="42">
         <v>2013</v>
       </c>
-      <c r="S3" s="47">
+      <c r="S3" s="42">
         <v>2014</v>
       </c>
-      <c r="T3" s="47">
+      <c r="T3" s="42">
         <v>2015</v>
       </c>
-      <c r="U3" s="47">
+      <c r="U3" s="42">
         <v>2016</v>
       </c>
-      <c r="V3" s="47">
+      <c r="V3" s="42">
         <v>2017</v>
       </c>
-      <c r="W3" s="47">
+      <c r="W3" s="42">
         <v>2018</v>
       </c>
-      <c r="X3" s="45">
+      <c r="X3" s="41">
         <v>2019</v>
       </c>
-      <c r="Y3" s="49">
+      <c r="Y3" s="44">
         <v>2020</v>
       </c>
     </row>
@@ -4121,70 +4004,70 @@
       <c r="A4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="8">
         <v>303918.51</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="8">
         <v>309575.40000000002</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="8">
         <v>300384.71999999997</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="8">
         <v>313574.71000000002</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="8">
         <v>328615.86</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="8">
         <v>329369.34999999998</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="8">
         <v>342812.72</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="8">
         <v>338694.07</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="8">
         <v>332869.05</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="8">
         <v>335505.55</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="8">
         <v>342817.43</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="8">
         <v>326094.38</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="8">
         <v>304024.53999999998</v>
       </c>
-      <c r="O4" s="25">
+      <c r="O4" s="8">
         <v>314307.58</v>
       </c>
-      <c r="P4" s="25">
+      <c r="P4" s="8">
         <v>311964.24</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4" s="8">
         <v>328315.46999999997</v>
       </c>
-      <c r="R4" s="25">
+      <c r="R4" s="8">
         <v>331764.81</v>
       </c>
-      <c r="S4" s="25">
+      <c r="S4" s="8">
         <v>313819.75</v>
       </c>
-      <c r="T4" s="25">
+      <c r="T4" s="8">
         <v>301927.02</v>
       </c>
-      <c r="U4" s="25">
+      <c r="U4" s="8">
         <v>297784.31</v>
       </c>
-      <c r="V4" s="25">
+      <c r="V4" s="8">
         <v>276487.67</v>
       </c>
-      <c r="W4" s="25">
+      <c r="W4" s="8">
         <v>262191.39</v>
       </c>
     </row>
@@ -4192,70 +4075,70 @@
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="11">
         <v>71642</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="10">
         <v>71352.09</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="10">
         <v>86513.41</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="10">
         <v>91192.44</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="10">
         <v>85717.27</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="10">
         <v>100063.75</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="10">
         <v>92920.16</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="10">
         <v>102061.53</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="10">
         <v>112056.48</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="10">
         <v>103321.36</v>
       </c>
-      <c r="L5" s="33">
+      <c r="L5" s="10">
         <v>109417.34</v>
       </c>
-      <c r="M5" s="33">
+      <c r="M5" s="10">
         <v>92294.76</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="10">
         <v>76684.149999999994</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5" s="10">
         <v>59890.67</v>
       </c>
-      <c r="P5" s="33">
+      <c r="P5" s="10">
         <v>73853.34</v>
       </c>
-      <c r="Q5" s="33">
+      <c r="Q5" s="10">
         <v>78699.759999999995</v>
       </c>
-      <c r="R5" s="33">
+      <c r="R5" s="10">
         <v>58777.760000000002</v>
       </c>
-      <c r="S5" s="33">
+      <c r="S5" s="10">
         <v>62869.27</v>
       </c>
-      <c r="T5" s="33">
+      <c r="T5" s="10">
         <v>73527.679999999993</v>
       </c>
-      <c r="U5" s="33">
+      <c r="U5" s="10">
         <v>58218.68</v>
       </c>
-      <c r="V5" s="33">
+      <c r="V5" s="10">
         <v>68256.399999999994</v>
       </c>
-      <c r="W5" s="33">
+      <c r="W5" s="10">
         <v>59000.95</v>
       </c>
     </row>
@@ -4271,76 +4154,76 @@
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="42">
         <v>1997</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="42">
         <v>1998</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="42">
         <v>1999</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="42">
         <v>2000</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="42">
         <v>2001</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="42">
         <v>2002</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="42">
         <v>2003</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="42">
         <v>2004</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="42">
         <v>2005</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="42">
         <v>2006</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="42">
         <v>2007</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="42">
         <v>2008</v>
       </c>
-      <c r="N8" s="47">
+      <c r="N8" s="42">
         <v>2009</v>
       </c>
-      <c r="O8" s="47">
+      <c r="O8" s="42">
         <v>2010</v>
       </c>
-      <c r="P8" s="47">
+      <c r="P8" s="42">
         <v>2011</v>
       </c>
-      <c r="Q8" s="47">
+      <c r="Q8" s="42">
         <v>2012</v>
       </c>
-      <c r="R8" s="47">
+      <c r="R8" s="42">
         <v>2013</v>
       </c>
-      <c r="S8" s="47">
+      <c r="S8" s="42">
         <v>2014</v>
       </c>
-      <c r="T8" s="47">
+      <c r="T8" s="42">
         <v>2015</v>
       </c>
-      <c r="U8" s="47">
+      <c r="U8" s="42">
         <v>2016</v>
       </c>
-      <c r="V8" s="47">
+      <c r="V8" s="42">
         <v>2017</v>
       </c>
-      <c r="W8" s="47">
+      <c r="W8" s="42">
         <v>2018</v>
       </c>
-      <c r="X8" s="45">
+      <c r="X8" s="41">
         <v>2019</v>
       </c>
-      <c r="Y8" s="49">
+      <c r="Y8" s="44">
         <v>2020</v>
       </c>
     </row>
@@ -4510,76 +4393,76 @@
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="42">
         <v>1997</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="42">
         <v>1998</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="42">
         <v>1999</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="42">
         <v>2000</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="42">
         <v>2001</v>
       </c>
-      <c r="G13" s="47">
+      <c r="G13" s="42">
         <v>2002</v>
       </c>
-      <c r="H13" s="47">
+      <c r="H13" s="42">
         <v>2003</v>
       </c>
-      <c r="I13" s="47">
+      <c r="I13" s="42">
         <v>2004</v>
       </c>
-      <c r="J13" s="47">
+      <c r="J13" s="42">
         <v>2005</v>
       </c>
-      <c r="K13" s="47">
+      <c r="K13" s="42">
         <v>2006</v>
       </c>
-      <c r="L13" s="47">
+      <c r="L13" s="42">
         <v>2007</v>
       </c>
-      <c r="M13" s="47">
+      <c r="M13" s="42">
         <v>2008</v>
       </c>
-      <c r="N13" s="47">
+      <c r="N13" s="42">
         <v>2009</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="42">
         <v>2010</v>
       </c>
-      <c r="P13" s="47">
+      <c r="P13" s="42">
         <v>2011</v>
       </c>
-      <c r="Q13" s="47">
+      <c r="Q13" s="42">
         <v>2012</v>
       </c>
-      <c r="R13" s="47">
+      <c r="R13" s="42">
         <v>2013</v>
       </c>
-      <c r="S13" s="47">
+      <c r="S13" s="42">
         <v>2014</v>
       </c>
-      <c r="T13" s="47">
+      <c r="T13" s="42">
         <v>2015</v>
       </c>
-      <c r="U13" s="47">
+      <c r="U13" s="42">
         <v>2016</v>
       </c>
-      <c r="V13" s="47">
+      <c r="V13" s="42">
         <v>2017</v>
       </c>
-      <c r="W13" s="47">
+      <c r="W13" s="42">
         <v>2018</v>
       </c>
-      <c r="X13" s="45">
+      <c r="X13" s="41">
         <v>2019</v>
       </c>
-      <c r="Y13" s="49">
+      <c r="Y13" s="44">
         <v>2020</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add BP 2022 primary energy data into our spreadsheet
</commit_message>
<xml_diff>
--- a/data/Germany & Spain Data.xlsx
+++ b/data/Germany & Spain Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trtim/Develop/germany-and-spain/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA57CFB8-6615-5442-B1B6-FF0C99AE94C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C0F2C5-204C-5645-8ABF-D0C48A99C3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10640" windowWidth="33720" windowHeight="10960" activeTab="3" xr2:uid="{FE379562-162F-468A-B10D-43820705E65E}"/>
+    <workbookView xWindow="0" yWindow="10640" windowWidth="37060" windowHeight="10960" activeTab="4" xr2:uid="{FE379562-162F-468A-B10D-43820705E65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="5" r:id="rId1"/>
     <sheet name="Industry" sheetId="1" r:id="rId2"/>
     <sheet name="Transport" sheetId="2" r:id="rId3"/>
     <sheet name="Power" sheetId="3" r:id="rId4"/>
+    <sheet name="Primary energy" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="41">
   <si>
     <t>TIME</t>
   </si>
@@ -179,18 +180,56 @@
   <si>
     <t>Germany</t>
   </si>
+  <si>
+    <t>EJ</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Hydro</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Biofuel</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>PJ</t>
+  </si>
+  <si>
+    <t>Renewables</t>
+  </si>
+  <si>
+    <t>Other renewables</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0.##########"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="[&gt;0.005]0.00;[=0]\-;\^"/>
+    <numFmt numFmtId="169" formatCode="[&gt;0.05]0.0;[=0]\-;\^"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +310,17 @@
     <font>
       <sz val="9"/>
       <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -411,14 +461,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -550,11 +601,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 18" xfId="4" xr:uid="{06ACEDC1-5CC0-E442-87B3-98D4C02855F7}"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{05A62228-BAA6-46A3-88C0-5B6930D4B7CE}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{31724FA5-7847-FE45-BD56-648C79BA1B58}"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
     <cellStyle name="Standard 2" xfId="3" xr:uid="{629DA393-64FF-480E-B039-636939B18E9E}"/>
   </cellStyles>
@@ -896,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A318FC36-9A92-4E6E-ACE0-025499D7FA26}">
   <dimension ref="A3:AB24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3902,7 +3966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712A49B1-B69A-4BE2-A124-7AF0E08088AC}">
   <dimension ref="A2:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14:Y15"/>
     </sheetView>
   </sheetViews>
@@ -4624,4 +4688,3114 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3FA813-0443-284D-9598-5B25F7394507}">
+  <dimension ref="A1:Z54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="Z57" sqref="Z57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C2" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D2" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E2" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G2" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H2" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I2" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J2" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K2" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L2" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M2" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N2" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O2" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P2" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q2" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R2" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S2" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T2" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U2" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V2" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W2" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X2" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y2" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z2" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="49">
+        <v>3.660545736</v>
+      </c>
+      <c r="C3" s="49">
+        <v>3.5730443624000001</v>
+      </c>
+      <c r="D3" s="49">
+        <v>3.4400939888000002</v>
+      </c>
+      <c r="E3" s="49">
+        <v>3.5715449888000004</v>
+      </c>
+      <c r="F3" s="49">
+        <v>3.581769736</v>
+      </c>
+      <c r="G3" s="49">
+        <v>3.5897357360000002</v>
+      </c>
+      <c r="H3" s="49">
+        <v>3.649031736</v>
+      </c>
+      <c r="I3" s="49">
+        <v>3.5571960449999995</v>
+      </c>
+      <c r="J3" s="49">
+        <v>3.4033940744</v>
+      </c>
+      <c r="K3" s="49">
+        <v>3.5399205618000003</v>
+      </c>
+      <c r="L3" s="49">
+        <v>3.6298322070000002</v>
+      </c>
+      <c r="M3" s="49">
+        <v>3.3545096320000001</v>
+      </c>
+      <c r="N3" s="49">
+        <v>3.0034527709999992</v>
+      </c>
+      <c r="O3" s="49">
+        <v>3.2262200000000001</v>
+      </c>
+      <c r="P3" s="49">
+        <v>3.278848</v>
+      </c>
+      <c r="Q3" s="49">
+        <v>3.3698670000000002</v>
+      </c>
+      <c r="R3" s="49">
+        <v>3.468235</v>
+      </c>
+      <c r="S3" s="49">
+        <v>3.3332219999999997</v>
+      </c>
+      <c r="T3" s="49">
+        <v>3.2942010000000002</v>
+      </c>
+      <c r="U3" s="49">
+        <v>3.2037659999999999</v>
+      </c>
+      <c r="V3" s="49">
+        <v>3.0093469999999996</v>
+      </c>
+      <c r="W3" s="49">
+        <v>2.9040839999999997</v>
+      </c>
+      <c r="X3" s="49">
+        <v>2.2471840000000003</v>
+      </c>
+      <c r="Y3" s="49">
+        <v>1.8060999999999998</v>
+      </c>
+      <c r="Z3" s="50">
+        <v>2.1155999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="49">
+        <v>0.76848714000000007</v>
+      </c>
+      <c r="C4" s="49">
+        <v>0.73231318800000011</v>
+      </c>
+      <c r="D4" s="49">
+        <v>0.82073840400000009</v>
+      </c>
+      <c r="E4" s="49">
+        <v>0.87654844799999998</v>
+      </c>
+      <c r="F4" s="49">
+        <v>0.80252582400000005</v>
+      </c>
+      <c r="G4" s="49">
+        <v>0.90426506400000006</v>
+      </c>
+      <c r="H4" s="49">
+        <v>0.842760972</v>
+      </c>
+      <c r="I4" s="49">
+        <v>0.88127953199999998</v>
+      </c>
+      <c r="J4" s="49">
+        <v>0.85883828400000006</v>
+      </c>
+      <c r="K4" s="49">
+        <v>0.74977214400000003</v>
+      </c>
+      <c r="L4" s="49">
+        <v>0.83890911600000007</v>
+      </c>
+      <c r="M4" s="49">
+        <v>0.565385472</v>
+      </c>
+      <c r="N4" s="49">
+        <v>0.39481524000000001</v>
+      </c>
+      <c r="O4" s="49">
+        <v>0.28876359600000001</v>
+      </c>
+      <c r="P4" s="49">
+        <v>0.53553358800000006</v>
+      </c>
+      <c r="Q4" s="49">
+        <v>0.64861905600000003</v>
+      </c>
+      <c r="R4" s="49">
+        <v>0.47716959600000003</v>
+      </c>
+      <c r="S4" s="49">
+        <v>0.48730165200000003</v>
+      </c>
+      <c r="T4" s="49">
+        <v>0.57302268579750115</v>
+      </c>
+      <c r="U4" s="49">
+        <v>0.43945238951999999</v>
+      </c>
+      <c r="V4" s="49">
+        <v>0.56307519576000009</v>
+      </c>
+      <c r="W4" s="49">
+        <v>0.48247875147599995</v>
+      </c>
+      <c r="X4" s="49">
+        <v>0.21234268922399999</v>
+      </c>
+      <c r="Y4" s="49">
+        <v>0.123789733956</v>
+      </c>
+      <c r="Z4" s="50">
+        <v>0.1608005136079676</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C7" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D7" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E7" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F7" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G7" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H7" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I7" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J7" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K7" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L7" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M7" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N7" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O7" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P7" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q7" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R7" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S7" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T7" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U7" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V7" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W7" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X7" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y7" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z7" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="49">
+        <v>5.9361375864607258</v>
+      </c>
+      <c r="C8" s="49">
+        <v>5.9425818883542174</v>
+      </c>
+      <c r="D8" s="49">
+        <v>5.7639861403089574</v>
+      </c>
+      <c r="E8" s="49">
+        <v>5.6535652797189497</v>
+      </c>
+      <c r="F8" s="49">
+        <v>5.727468239673307</v>
+      </c>
+      <c r="G8" s="49">
+        <v>5.5360078633064003</v>
+      </c>
+      <c r="H8" s="49">
+        <v>5.4277814338780903</v>
+      </c>
+      <c r="I8" s="49">
+        <v>5.3657644862539664</v>
+      </c>
+      <c r="J8" s="49">
+        <v>5.2562073672151479</v>
+      </c>
+      <c r="K8" s="49">
+        <v>5.2460538380265138</v>
+      </c>
+      <c r="L8" s="49">
+        <v>4.7500508109785944</v>
+      </c>
+      <c r="M8" s="49">
+        <v>5.0366496430546395</v>
+      </c>
+      <c r="N8" s="49">
+        <v>4.8234181241768992</v>
+      </c>
+      <c r="O8" s="49">
+        <v>4.8875193710000007</v>
+      </c>
+      <c r="P8" s="49">
+        <v>4.727774966000001</v>
+      </c>
+      <c r="Q8" s="49">
+        <v>4.6994014380000007</v>
+      </c>
+      <c r="R8" s="49">
+        <v>4.8033446200000007</v>
+      </c>
+      <c r="S8" s="49">
+        <v>4.6739449520000012</v>
+      </c>
+      <c r="T8" s="49">
+        <v>4.6675521479999995</v>
+      </c>
+      <c r="U8" s="49">
+        <v>4.7639474210000001</v>
+      </c>
+      <c r="V8" s="49">
+        <v>4.8673545697095957</v>
+      </c>
+      <c r="W8" s="49">
+        <v>4.6320574056674024</v>
+      </c>
+      <c r="X8" s="49">
+        <v>4.6610522749930396</v>
+      </c>
+      <c r="Y8" s="49">
+        <v>4.2202221482290811</v>
+      </c>
+      <c r="Z8" s="50">
+        <v>4.1840938220687356</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="49">
+        <v>2.6094154931835458</v>
+      </c>
+      <c r="C9" s="49">
+        <v>2.8281579850517695</v>
+      </c>
+      <c r="D9" s="49">
+        <v>2.926544074136582</v>
+      </c>
+      <c r="E9" s="49">
+        <v>2.9650195439620624</v>
+      </c>
+      <c r="F9" s="49">
+        <v>3.0893487626058636</v>
+      </c>
+      <c r="G9" s="49">
+        <v>3.114871987901175</v>
+      </c>
+      <c r="H9" s="49">
+        <v>3.1885755904589561</v>
+      </c>
+      <c r="I9" s="49">
+        <v>3.2637854901822276</v>
+      </c>
+      <c r="J9" s="49">
+        <v>3.2919190802392424</v>
+      </c>
+      <c r="K9" s="49">
+        <v>3.3137542409686715</v>
+      </c>
+      <c r="L9" s="49">
+        <v>3.3382690202651082</v>
+      </c>
+      <c r="M9" s="49">
+        <v>3.2225958865485529</v>
+      </c>
+      <c r="N9" s="49">
+        <v>3.0235130192400321</v>
+      </c>
+      <c r="O9" s="49">
+        <v>2.9423522334426937</v>
+      </c>
+      <c r="P9" s="49">
+        <v>2.8079899102634829</v>
+      </c>
+      <c r="Q9" s="49">
+        <v>2.6246443045224672</v>
+      </c>
+      <c r="R9" s="49">
+        <v>2.4670060498765243</v>
+      </c>
+      <c r="S9" s="49">
+        <v>2.4605660048874753</v>
+      </c>
+      <c r="T9" s="49">
+        <v>2.5434828407206962</v>
+      </c>
+      <c r="U9" s="49">
+        <v>2.6287619365395645</v>
+      </c>
+      <c r="V9" s="49">
+        <v>2.6423500768914261</v>
+      </c>
+      <c r="W9" s="49">
+        <v>2.6930054546157036</v>
+      </c>
+      <c r="X9" s="49">
+        <v>2.6954231210078263</v>
+      </c>
+      <c r="Y9" s="49">
+        <v>2.2142806696342023</v>
+      </c>
+      <c r="Z9" s="50">
+        <v>2.4504481154547921</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C12" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D12" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E12" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F12" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G12" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H12" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I12" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J12" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K12" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L12" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M12" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N12" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O12" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P12" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q12" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R12" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S12" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T12" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U12" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V12" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W12" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X12" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y12" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z12" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="49">
+        <v>2.9917210000000001</v>
+      </c>
+      <c r="C13" s="49">
+        <v>3.0191410000000003</v>
+      </c>
+      <c r="D13" s="49">
+        <v>3.0102870000000004</v>
+      </c>
+      <c r="E13" s="49">
+        <v>2.9852849999999993</v>
+      </c>
+      <c r="F13" s="49">
+        <v>3.1481350000000008</v>
+      </c>
+      <c r="G13" s="49">
+        <v>3.1432600000000002</v>
+      </c>
+      <c r="H13" s="49">
+        <v>3.1813910000000001</v>
+      </c>
+      <c r="I13" s="49">
+        <v>3.1975579999999999</v>
+      </c>
+      <c r="J13" s="49">
+        <v>3.2501177710106353</v>
+      </c>
+      <c r="K13" s="49">
+        <v>3.3122482735877967</v>
+      </c>
+      <c r="L13" s="49">
+        <v>3.1909030508088567</v>
+      </c>
+      <c r="M13" s="49">
+        <v>3.2220226911707877</v>
+      </c>
+      <c r="N13" s="49">
+        <v>3.0394843792871828</v>
+      </c>
+      <c r="O13" s="49">
+        <v>3.1705649999999999</v>
+      </c>
+      <c r="P13" s="49">
+        <v>2.9109860000000003</v>
+      </c>
+      <c r="Q13" s="49">
+        <v>2.9199620000000004</v>
+      </c>
+      <c r="R13" s="49">
+        <v>3.0590760000000001</v>
+      </c>
+      <c r="S13" s="49">
+        <v>2.6602210000000004</v>
+      </c>
+      <c r="T13" s="49">
+        <v>2.7703300000000004</v>
+      </c>
+      <c r="U13" s="49">
+        <v>3.0558510000000005</v>
+      </c>
+      <c r="V13" s="49">
+        <v>3.1585850000000004</v>
+      </c>
+      <c r="W13" s="49">
+        <v>3.0906260000000008</v>
+      </c>
+      <c r="X13" s="49">
+        <v>3.2141889999999993</v>
+      </c>
+      <c r="Y13" s="49">
+        <v>3.1360500000000004</v>
+      </c>
+      <c r="Z13" s="50">
+        <v>3.2590911961722484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="49">
+        <v>0.47336032159819214</v>
+      </c>
+      <c r="C14" s="49">
+        <v>0.48595340124691211</v>
+      </c>
+      <c r="D14" s="49">
+        <v>0.55629108256032</v>
+      </c>
+      <c r="E14" s="49">
+        <v>0.63707035703155213</v>
+      </c>
+      <c r="F14" s="49">
+        <v>0.68649965687174408</v>
+      </c>
+      <c r="G14" s="49">
+        <v>0.78492364008408011</v>
+      </c>
+      <c r="H14" s="49">
+        <v>0.89383420780704015</v>
+      </c>
+      <c r="I14" s="49">
+        <v>1.0536866846513282</v>
+      </c>
+      <c r="J14" s="49">
+        <v>1.24927039406232</v>
+      </c>
+      <c r="K14" s="49">
+        <v>1.3074253168645444</v>
+      </c>
+      <c r="L14" s="49">
+        <v>1.3304617893252</v>
+      </c>
+      <c r="M14" s="49">
+        <v>1.4613182391169444</v>
+      </c>
+      <c r="N14" s="49">
+        <v>1.3070779836209283</v>
+      </c>
+      <c r="O14" s="49">
+        <v>1.3030728533946723</v>
+      </c>
+      <c r="P14" s="49">
+        <v>1.2112589997357124</v>
+      </c>
+      <c r="Q14" s="49">
+        <v>1.1961221089996801</v>
+      </c>
+      <c r="R14" s="49">
+        <v>1.0918114571869919</v>
+      </c>
+      <c r="S14" s="49">
+        <v>0.99086039719200014</v>
+      </c>
+      <c r="T14" s="49">
+        <v>1.0275762048480002</v>
+      </c>
+      <c r="U14" s="49">
+        <v>1.048377399552</v>
+      </c>
+      <c r="V14" s="49">
+        <v>1.1416361086800004</v>
+      </c>
+      <c r="W14" s="49">
+        <v>1.1339009956800004</v>
+      </c>
+      <c r="X14" s="49">
+        <v>1.2950810726400002</v>
+      </c>
+      <c r="Y14" s="49">
+        <v>1.1696483127600004</v>
+      </c>
+      <c r="Z14" s="50">
+        <v>1.2203513541760358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C17" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D17" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E17" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F17" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G17" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H17" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I17" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J17" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K17" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L17" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M17" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N17" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O17" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P17" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q17" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R17" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S17" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T17" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U17" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V17" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W17" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X17" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y17" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z17" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="49">
+        <v>0.20174709677419356</v>
+      </c>
+      <c r="C18" s="49">
+        <v>0.2022793548387096</v>
+      </c>
+      <c r="D18" s="49">
+        <v>0.22020580645161289</v>
+      </c>
+      <c r="E18" s="49">
+        <v>0.26506451612903226</v>
+      </c>
+      <c r="F18" s="49">
+        <v>0.24536405529953911</v>
+      </c>
+      <c r="G18" s="49">
+        <v>0.24903496357960461</v>
+      </c>
+      <c r="H18" s="49">
+        <v>0.19128148391668737</v>
+      </c>
+      <c r="I18" s="49">
+        <v>0.21521502216318053</v>
+      </c>
+      <c r="J18" s="49">
+        <v>0.20243418129848909</v>
+      </c>
+      <c r="K18" s="49">
+        <v>0.20518668898356654</v>
+      </c>
+      <c r="L18" s="49">
+        <v>0.21549864919354825</v>
+      </c>
+      <c r="M18" s="49">
+        <v>0.20680566419555185</v>
+      </c>
+      <c r="N18" s="49">
+        <v>0.19133317204301062</v>
+      </c>
+      <c r="O18" s="49">
+        <v>0.20936413417771604</v>
+      </c>
+      <c r="P18" s="49">
+        <v>0.17549346774193539</v>
+      </c>
+      <c r="Q18" s="49">
+        <v>0.21474290322580628</v>
+      </c>
+      <c r="R18" s="49">
+        <v>0.22564497085114638</v>
+      </c>
+      <c r="S18" s="49">
+        <v>0.19102716438091541</v>
+      </c>
+      <c r="T18" s="49">
+        <v>0.18397633064516111</v>
+      </c>
+      <c r="U18" s="49">
+        <v>0.19800869249856823</v>
+      </c>
+      <c r="V18" s="49">
+        <v>0.19304999999999997</v>
+      </c>
+      <c r="W18" s="49">
+        <v>0.16851906621392193</v>
+      </c>
+      <c r="X18" s="49">
+        <v>0.18723733636399675</v>
+      </c>
+      <c r="Y18" s="49">
+        <v>0.17322793627386462</v>
+      </c>
+      <c r="Z18" s="50">
+        <v>0.17992270658148471</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="49">
+        <v>0.37021741935483876</v>
+      </c>
+      <c r="C19" s="49">
+        <v>0.36198870967741931</v>
+      </c>
+      <c r="D19" s="49">
+        <v>0.24338032258064513</v>
+      </c>
+      <c r="E19" s="49">
+        <v>0.31477741935483866</v>
+      </c>
+      <c r="F19" s="49">
+        <v>0.43390306451612909</v>
+      </c>
+      <c r="G19" s="49">
+        <v>0.24083887617065558</v>
+      </c>
+      <c r="H19" s="49">
+        <v>0.42862209677419344</v>
+      </c>
+      <c r="I19" s="49">
+        <v>0.32860514485309222</v>
+      </c>
+      <c r="J19" s="49">
+        <v>0.18422974275214363</v>
+      </c>
+      <c r="K19" s="49">
+        <v>0.26520310407790615</v>
+      </c>
+      <c r="L19" s="49">
+        <v>0.27721656653225796</v>
+      </c>
+      <c r="M19" s="49">
+        <v>0.23805463434181515</v>
+      </c>
+      <c r="N19" s="49">
+        <v>0.2649415789470736</v>
+      </c>
+      <c r="O19" s="49">
+        <v>0.42002420374145449</v>
+      </c>
+      <c r="P19" s="49">
+        <v>0.30385366639285799</v>
+      </c>
+      <c r="Q19" s="49">
+        <v>0.20279903225806437</v>
+      </c>
+      <c r="R19" s="49">
+        <v>0.36086612304992366</v>
+      </c>
+      <c r="S19" s="49">
+        <v>0.38200556499903376</v>
+      </c>
+      <c r="T19" s="49">
+        <v>0.27280887096774176</v>
+      </c>
+      <c r="U19" s="49">
+        <v>0.35065994865241751</v>
+      </c>
+      <c r="V19" s="49">
+        <v>0.17553658064516126</v>
+      </c>
+      <c r="W19" s="49">
+        <v>0.32701823429541588</v>
+      </c>
+      <c r="X19" s="49">
+        <v>0.21338164405893933</v>
+      </c>
+      <c r="Y19" s="49">
+        <v>0.2884301630441079</v>
+      </c>
+      <c r="Z19" s="50">
+        <v>0.27851679375425786</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C22" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D22" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E22" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F22" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G22" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H22" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I22" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J22" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K22" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L22" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M22" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N22" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O22" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P22" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q22" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R22" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S22" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T22" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U22" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V22" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W22" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X22" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y22" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z22" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="49">
+        <v>1.7399096774193548</v>
+      </c>
+      <c r="C23" s="49">
+        <v>1.6507526881720427</v>
+      </c>
+      <c r="D23" s="49">
+        <v>1.7365999999999997</v>
+      </c>
+      <c r="E23" s="49">
+        <v>1.7325344086021508</v>
+      </c>
+      <c r="F23" s="49">
+        <v>1.7385268642647673</v>
+      </c>
+      <c r="G23" s="49">
+        <v>1.6621425390218518</v>
+      </c>
+      <c r="H23" s="49">
+        <v>1.6536718362282872</v>
+      </c>
+      <c r="I23" s="49">
+        <v>1.6630982638175462</v>
+      </c>
+      <c r="J23" s="49">
+        <v>1.6127479685585948</v>
+      </c>
+      <c r="K23" s="49">
+        <v>1.6450391965915996</v>
+      </c>
+      <c r="L23" s="49">
+        <v>1.3727565120967733</v>
+      </c>
+      <c r="M23" s="49">
+        <v>1.4442487778000388</v>
+      </c>
+      <c r="N23" s="49">
+        <v>1.3017633213859012</v>
+      </c>
+      <c r="O23" s="49">
+        <v>1.3477019988125856</v>
+      </c>
+      <c r="P23" s="49">
+        <v>1.0289547498328082</v>
+      </c>
+      <c r="Q23" s="49">
+        <v>0.9420991202346034</v>
+      </c>
+      <c r="R23" s="49">
+        <v>0.91599310143800938</v>
+      </c>
+      <c r="S23" s="49">
+        <v>0.90900136179254298</v>
+      </c>
+      <c r="T23" s="49">
+        <v>0.85388762825460729</v>
+      </c>
+      <c r="U23" s="49">
+        <v>0.78269423286791273</v>
+      </c>
+      <c r="V23" s="49">
+        <v>0.70169207462903205</v>
+      </c>
+      <c r="W23" s="49">
+        <v>0.69466754516129026</v>
+      </c>
+      <c r="X23" s="49">
+        <v>0.6836051638417181</v>
+      </c>
+      <c r="Y23" s="49">
+        <v>0.58411802097169185</v>
+      </c>
+      <c r="Z23" s="50">
+        <v>0.62372063125582122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="49">
+        <v>0.56487204301075278</v>
+      </c>
+      <c r="C24" s="49">
+        <v>0.6026166666666668</v>
+      </c>
+      <c r="D24" s="49">
+        <v>0.60117634408602161</v>
+      </c>
+      <c r="E24" s="49">
+        <v>0.63543763440860213</v>
+      </c>
+      <c r="F24" s="49">
+        <v>0.64655479681608707</v>
+      </c>
+      <c r="G24" s="49">
+        <v>0.63540586888657624</v>
+      </c>
+      <c r="H24" s="49">
+        <v>0.61990151985111652</v>
+      </c>
+      <c r="I24" s="49">
+        <v>0.63318485720156137</v>
+      </c>
+      <c r="J24" s="49">
+        <v>0.56916385259289493</v>
+      </c>
+      <c r="K24" s="49">
+        <v>0.59101332927571493</v>
+      </c>
+      <c r="L24" s="49">
+        <v>0.53825410282258046</v>
+      </c>
+      <c r="M24" s="49">
+        <v>0.572478831897415</v>
+      </c>
+      <c r="N24" s="49">
+        <v>0.50901732078853024</v>
+      </c>
+      <c r="O24" s="49">
+        <v>0.5907716663368292</v>
+      </c>
+      <c r="P24" s="49">
+        <v>0.55017052512771403</v>
+      </c>
+      <c r="Q24" s="49">
+        <v>0.58225249266862111</v>
+      </c>
+      <c r="R24" s="49">
+        <v>0.53413002018072231</v>
+      </c>
+      <c r="S24" s="49">
+        <v>0.53630041529843508</v>
+      </c>
+      <c r="T24" s="49">
+        <v>0.53310815092165842</v>
+      </c>
+      <c r="U24" s="49">
+        <v>0.54210510394963851</v>
+      </c>
+      <c r="V24" s="49">
+        <v>0.5342557035967741</v>
+      </c>
+      <c r="W24" s="49">
+        <v>0.50968924731182785</v>
+      </c>
+      <c r="X24" s="49">
+        <v>0.53067712380792287</v>
+      </c>
+      <c r="Y24" s="49">
+        <v>0.52892946951415398</v>
+      </c>
+      <c r="Z24" s="50">
+        <v>0.5107670742274929</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24"/>
+      <c r="Z26" s="24"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C27" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D27" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E27" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F27" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G27" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H27" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I27" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J27" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K27" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L27" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M27" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N27" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O27" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P27" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q27" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R27" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S27" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T27" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U27" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V27" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W27" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X27" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y27" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z27" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="51">
+        <v>3.3249443050516998</v>
+      </c>
+      <c r="C28" s="51">
+        <v>3.6937775909186468</v>
+      </c>
+      <c r="D28" s="51">
+        <v>4.8093412763626402</v>
+      </c>
+      <c r="E28" s="51">
+        <v>9.2493486030175536</v>
+      </c>
+      <c r="F28" s="51">
+        <v>12.94935717122245</v>
+      </c>
+      <c r="G28" s="51">
+        <v>20.348220531654423</v>
+      </c>
+      <c r="H28" s="51">
+        <v>29.155955751745488</v>
+      </c>
+      <c r="I28" s="51">
+        <v>38.863366324139548</v>
+      </c>
+      <c r="J28" s="51">
+        <v>71.783416667577484</v>
+      </c>
+      <c r="K28" s="51">
+        <v>114.47551528397938</v>
+      </c>
+      <c r="L28" s="51">
+        <v>130.12707510781803</v>
+      </c>
+      <c r="M28" s="51">
+        <v>114.17504556898903</v>
+      </c>
+      <c r="N28" s="51">
+        <v>113.44531941092723</v>
+      </c>
+      <c r="O28" s="51">
+        <v>113.55200000000002</v>
+      </c>
+      <c r="P28" s="51">
+        <v>118.254</v>
+      </c>
+      <c r="Q28" s="51">
+        <v>125.97320000000001</v>
+      </c>
+      <c r="R28" s="51">
+        <v>112.72300000000001</v>
+      </c>
+      <c r="S28" s="51">
+        <v>118.19280000000002</v>
+      </c>
+      <c r="T28" s="51">
+        <v>110.8014</v>
+      </c>
+      <c r="U28" s="51">
+        <v>111.04</v>
+      </c>
+      <c r="V28" s="51">
+        <v>112.9996</v>
+      </c>
+      <c r="W28" s="51">
+        <v>117.78444564000002</v>
+      </c>
+      <c r="X28" s="51">
+        <v>115.77650818400001</v>
+      </c>
+      <c r="Y28" s="51">
+        <v>141.375622212</v>
+      </c>
+      <c r="Z28" s="52">
+        <v>124.51626466799999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="51">
+        <v>0</v>
+      </c>
+      <c r="C29" s="51">
+        <v>0</v>
+      </c>
+      <c r="D29" s="51">
+        <v>0</v>
+      </c>
+      <c r="E29" s="51">
+        <v>2.9710015387146678</v>
+      </c>
+      <c r="F29" s="51">
+        <v>2.9584970885112396</v>
+      </c>
+      <c r="G29" s="51">
+        <v>5.7674712735897318</v>
+      </c>
+      <c r="H29" s="51">
+        <v>7.9494199501957272</v>
+      </c>
+      <c r="I29" s="51">
+        <v>7.3255835301431551</v>
+      </c>
+      <c r="J29" s="51">
+        <v>10.589388745089714</v>
+      </c>
+      <c r="K29" s="51">
+        <v>7.0124062862476881</v>
+      </c>
+      <c r="L29" s="51">
+        <v>6.3632262172269058</v>
+      </c>
+      <c r="M29" s="51">
+        <v>8.3264514425865457</v>
+      </c>
+      <c r="N29" s="51">
+        <v>12.860989836367853</v>
+      </c>
+      <c r="O29" s="51">
+        <v>59.663487573505577</v>
+      </c>
+      <c r="P29" s="51">
+        <v>71.166463108481011</v>
+      </c>
+      <c r="Q29" s="51">
+        <v>87.889495459999921</v>
+      </c>
+      <c r="R29" s="51">
+        <v>38.029952380000005</v>
+      </c>
+      <c r="S29" s="51">
+        <v>40.112638132000008</v>
+      </c>
+      <c r="T29" s="51">
+        <v>41.07944530999999</v>
+      </c>
+      <c r="U29" s="51">
+        <v>46.582136350000013</v>
+      </c>
+      <c r="V29" s="51">
+        <v>54.62837300999999</v>
+      </c>
+      <c r="W29" s="51">
+        <v>70.280500030000013</v>
+      </c>
+      <c r="X29" s="51">
+        <v>70.138415464000005</v>
+      </c>
+      <c r="Y29" s="51">
+        <v>57.347654039999981</v>
+      </c>
+      <c r="Z29" s="52">
+        <v>54.835024290000007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+      <c r="Y31" s="24"/>
+      <c r="Z31" s="24"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C32" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D32" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E32" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F32" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G32" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H32" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I32" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J32" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K32" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L32" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M32" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N32" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O32" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P32" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q32" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R32" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S32" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T32" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U32" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V32" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W32" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X32" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y32" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z32" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="49">
+        <v>6.141256527279363E-2</v>
+      </c>
+      <c r="C33" s="49">
+        <v>8.2874664687692834E-2</v>
+      </c>
+      <c r="D33" s="49">
+        <v>9.7644341276362623E-2</v>
+      </c>
+      <c r="E33" s="49">
+        <v>0.14945096150624335</v>
+      </c>
+      <c r="F33" s="49">
+        <v>0.18481341247076158</v>
+      </c>
+      <c r="G33" s="49">
+        <v>0.2620214775555878</v>
+      </c>
+      <c r="H33" s="49">
+        <v>0.33453794072382981</v>
+      </c>
+      <c r="I33" s="49">
+        <v>0.43678371482681044</v>
+      </c>
+      <c r="J33" s="49">
+        <v>0.54057146178803461</v>
+      </c>
+      <c r="K33" s="49">
+        <v>0.67613523378671803</v>
+      </c>
+      <c r="L33" s="49">
+        <v>0.85728774849491451</v>
+      </c>
+      <c r="M33" s="49">
+        <v>0.90054416548483718</v>
+      </c>
+      <c r="N33" s="49">
+        <v>0.93239698906445123</v>
+      </c>
+      <c r="O33" s="49">
+        <v>1.008370175341381</v>
+      </c>
+      <c r="P33" s="49">
+        <v>1.236053578088119</v>
+      </c>
+      <c r="Q33" s="49">
+        <v>1.396820655278592</v>
+      </c>
+      <c r="R33" s="49">
+        <v>1.4543760232219194</v>
+      </c>
+      <c r="S33" s="49">
+        <v>1.5815634309155875</v>
+      </c>
+      <c r="T33" s="49">
+        <v>1.8323690843317959</v>
+      </c>
+      <c r="U33" s="49">
+        <v>1.8215751612903215</v>
+      </c>
+      <c r="V33" s="49">
+        <v>2.0752795435483873</v>
+      </c>
+      <c r="W33" s="49">
+        <v>2.1643043451872548</v>
+      </c>
+      <c r="X33" s="49">
+        <v>2.3094588591616971</v>
+      </c>
+      <c r="Y33" s="49">
+        <v>2.4368229481172006</v>
+      </c>
+      <c r="Z33" s="50">
+        <v>2.2792854464535846</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="49">
+        <v>2.4849798387096767E-2</v>
+      </c>
+      <c r="C34" s="49">
+        <v>3.2146088709677424E-2</v>
+      </c>
+      <c r="D34" s="49">
+        <v>4.9203387096774194E-2</v>
+      </c>
+      <c r="E34" s="49">
+        <v>7.0639751538714671E-2</v>
+      </c>
+      <c r="F34" s="49">
+        <v>9.3439101927220922E-2</v>
+      </c>
+      <c r="G34" s="49">
+        <v>0.13396475899471355</v>
+      </c>
+      <c r="H34" s="49">
+        <v>0.1710361941437441</v>
+      </c>
+      <c r="I34" s="49">
+        <v>0.20904563746480515</v>
+      </c>
+      <c r="J34" s="49">
+        <v>0.25978846336738448</v>
+      </c>
+      <c r="K34" s="49">
+        <v>0.27875182655405034</v>
+      </c>
+      <c r="L34" s="49">
+        <v>0.32546468589464617</v>
+      </c>
+      <c r="M34" s="49">
+        <v>0.40510091622920236</v>
+      </c>
+      <c r="N34" s="49">
+        <v>0.49393629221415303</v>
+      </c>
+      <c r="O34" s="49">
+        <v>0.61059175683055245</v>
+      </c>
+      <c r="P34" s="49">
+        <v>0.63065915232151815</v>
+      </c>
+      <c r="Q34" s="49">
+        <v>0.75153658942545831</v>
+      </c>
+      <c r="R34" s="49">
+        <v>0.77462409215957251</v>
+      </c>
+      <c r="S34" s="49">
+        <v>0.74295019534465778</v>
+      </c>
+      <c r="T34" s="49">
+        <v>0.71986530938910875</v>
+      </c>
+      <c r="U34" s="49">
+        <v>0.71455054433295639</v>
+      </c>
+      <c r="V34" s="49">
+        <v>0.73234598067096768</v>
+      </c>
+      <c r="W34" s="49">
+        <v>0.74739617617362253</v>
+      </c>
+      <c r="X34" s="49">
+        <v>0.78207806093150878</v>
+      </c>
+      <c r="Y34" s="49">
+        <v>0.85693150770137594</v>
+      </c>
+      <c r="Z34" s="50">
+        <v>0.97074632480982415</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A36" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="24"/>
+      <c r="W36" s="24"/>
+      <c r="X36" s="24"/>
+      <c r="Y36" s="24"/>
+      <c r="Z36" s="24"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C37" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D37" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E37" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F37" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G37" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H37" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I37" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J37" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K37" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L37" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M37" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N37" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O37" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P37" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q37" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R37" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S37" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T37" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U37" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V37" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W37" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X37" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y37" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z37" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="49">
+        <v>0</v>
+      </c>
+      <c r="C38" s="49">
+        <v>0</v>
+      </c>
+      <c r="D38" s="49">
+        <v>0</v>
+      </c>
+      <c r="E38" s="49">
+        <v>0</v>
+      </c>
+      <c r="F38" s="49">
+        <v>0</v>
+      </c>
+      <c r="G38" s="49">
+        <v>0</v>
+      </c>
+      <c r="H38" s="49">
+        <v>0</v>
+      </c>
+      <c r="I38" s="49">
+        <v>5.7782884733922329E-3</v>
+      </c>
+      <c r="J38" s="49">
+        <v>1.3483242139648834E-2</v>
+      </c>
+      <c r="K38" s="49">
+        <v>2.3201430310407781E-2</v>
+      </c>
+      <c r="L38" s="49">
+        <v>3.1932889112903214E-2</v>
+      </c>
+      <c r="M38" s="49">
+        <v>4.5603870967741912E-2</v>
+      </c>
+      <c r="N38" s="49">
+        <v>6.7511021505376287E-2</v>
+      </c>
+      <c r="O38" s="49">
+        <v>0.1195352998218879</v>
+      </c>
+      <c r="P38" s="49">
+        <v>0.19853375098347742</v>
+      </c>
+      <c r="Q38" s="49">
+        <v>0.2639891612903224</v>
+      </c>
+      <c r="R38" s="49">
+        <v>0.30043806645938564</v>
+      </c>
+      <c r="S38" s="49">
+        <v>0.33703562294765277</v>
+      </c>
+      <c r="T38" s="49">
+        <v>0.3603617108294927</v>
+      </c>
+      <c r="U38" s="49">
+        <v>0.35340108799389158</v>
+      </c>
+      <c r="V38" s="49">
+        <v>0.36303938709677419</v>
+      </c>
+      <c r="W38" s="49">
+        <v>0.41393037351443113</v>
+      </c>
+      <c r="X38" s="49">
+        <v>0.42117250518692761</v>
+      </c>
+      <c r="Y38" s="49">
+        <v>0.45988320315997361</v>
+      </c>
+      <c r="Z38" s="50">
+        <v>0.46158181269595561</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="49">
+        <v>0</v>
+      </c>
+      <c r="C39" s="49">
+        <v>0</v>
+      </c>
+      <c r="D39" s="49">
+        <v>0</v>
+      </c>
+      <c r="E39" s="49">
+        <v>0</v>
+      </c>
+      <c r="F39" s="49">
+        <v>0</v>
+      </c>
+      <c r="G39" s="49">
+        <v>0</v>
+      </c>
+      <c r="H39" s="49">
+        <v>0</v>
+      </c>
+      <c r="I39" s="49">
+        <v>0</v>
+      </c>
+      <c r="J39" s="49">
+        <v>0</v>
+      </c>
+      <c r="K39" s="49">
+        <v>0</v>
+      </c>
+      <c r="L39" s="49">
+        <v>5.1711532258064486E-3</v>
+      </c>
+      <c r="M39" s="49">
+        <v>2.6079587257062695E-2</v>
+      </c>
+      <c r="N39" s="49">
+        <v>6.0995526017182666E-2</v>
+      </c>
+      <c r="O39" s="49">
+        <v>7.0588363783095118E-2</v>
+      </c>
+      <c r="P39" s="49">
+        <v>8.6197833784241354E-2</v>
+      </c>
+      <c r="Q39" s="49">
+        <v>0.1181151062198357</v>
+      </c>
+      <c r="R39" s="49">
+        <v>0.12863754221518389</v>
+      </c>
+      <c r="S39" s="49">
+        <v>0.13334964725927309</v>
+      </c>
+      <c r="T39" s="49">
+        <v>0.13435332472350459</v>
+      </c>
+      <c r="U39" s="49">
+        <v>0.1314696444209088</v>
+      </c>
+      <c r="V39" s="49">
+        <v>0.13720126895129031</v>
+      </c>
+      <c r="W39" s="49">
+        <v>0.12138173174872663</v>
+      </c>
+      <c r="X39" s="49">
+        <v>0.14337009648322871</v>
+      </c>
+      <c r="Y39" s="49">
+        <v>0.19540040434247796</v>
+      </c>
+      <c r="Z39" s="50">
+        <v>0.25251419827760596</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A41" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="24"/>
+      <c r="W41" s="24"/>
+      <c r="X41" s="24"/>
+      <c r="Y41" s="24"/>
+      <c r="Z41" s="24"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C42" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D42" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E42" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F42" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G42" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H42" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I42" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J42" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K42" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L42" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M42" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N42" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O42" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P42" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q42" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R42" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S42" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T42" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U42" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V42" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W42" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X42" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y42" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z42" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A43" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="49">
+        <v>3.1573548387096764E-2</v>
+      </c>
+      <c r="C43" s="49">
+        <v>4.7786129032258061E-2</v>
+      </c>
+      <c r="D43" s="49">
+        <v>5.8846451612903229E-2</v>
+      </c>
+      <c r="E43" s="49">
+        <v>0.10112903225806449</v>
+      </c>
+      <c r="F43" s="49">
+        <v>0.11104838709677417</v>
+      </c>
+      <c r="G43" s="49">
+        <v>0.16602330905306972</v>
+      </c>
+      <c r="H43" s="49">
+        <v>0.19927680521091803</v>
+      </c>
+      <c r="I43" s="49">
+        <v>0.26991972673104569</v>
+      </c>
+      <c r="J43" s="49">
+        <v>0.2863024213964882</v>
+      </c>
+      <c r="K43" s="49">
+        <v>0.32086604990870343</v>
+      </c>
+      <c r="L43" s="49">
+        <v>0.41233839314516108</v>
+      </c>
+      <c r="M43" s="49">
+        <v>0.41865931677018609</v>
+      </c>
+      <c r="N43" s="49">
+        <v>0.39631935483870945</v>
+      </c>
+      <c r="O43" s="49">
+        <v>0.38516485849990084</v>
+      </c>
+      <c r="P43" s="49">
+        <v>0.49513767309205314</v>
+      </c>
+      <c r="Q43" s="49">
+        <v>0.5101316129032254</v>
+      </c>
+      <c r="R43" s="49">
+        <v>0.51742929071123156</v>
+      </c>
+      <c r="S43" s="49">
+        <v>0.57050676646706544</v>
+      </c>
+      <c r="T43" s="49">
+        <v>0.78162552995391621</v>
+      </c>
+      <c r="U43" s="49">
+        <v>0.7702543920595526</v>
+      </c>
+      <c r="V43" s="49">
+        <v>1.012607129032258</v>
+      </c>
+      <c r="W43" s="49">
+        <v>1.0472412733446517</v>
+      </c>
+      <c r="X43" s="49">
+        <v>1.1946711886984445</v>
+      </c>
+      <c r="Y43" s="49">
+        <v>1.2489770132982225</v>
+      </c>
+      <c r="Z43" s="50">
+        <v>1.1087383541696731</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="49">
+        <v>7.8987096774193553E-3</v>
+      </c>
+      <c r="C44" s="49">
+        <v>1.4392258064516134E-2</v>
+      </c>
+      <c r="D44" s="49">
+        <v>2.9210322580645161E-2</v>
+      </c>
+      <c r="E44" s="49">
+        <v>5.0319677419354843E-2</v>
+      </c>
+      <c r="F44" s="49">
+        <v>7.1483433179723499E-2</v>
+      </c>
+      <c r="G44" s="49">
+        <v>9.8163908428720068E-2</v>
+      </c>
+      <c r="H44" s="49">
+        <v>0.12606839330024813</v>
+      </c>
+      <c r="I44" s="49">
+        <v>0.16287096774193546</v>
+      </c>
+      <c r="J44" s="49">
+        <v>0.21828832993058386</v>
+      </c>
+      <c r="K44" s="49">
+        <v>0.23864181984175278</v>
+      </c>
+      <c r="L44" s="49">
+        <v>0.28062667741935471</v>
+      </c>
+      <c r="M44" s="49">
+        <v>0.33328862752955307</v>
+      </c>
+      <c r="N44" s="49">
+        <v>0.38090596072812588</v>
+      </c>
+      <c r="O44" s="49">
+        <v>0.43646778807181913</v>
+      </c>
+      <c r="P44" s="49">
+        <v>0.42140876671911848</v>
+      </c>
+      <c r="Q44" s="49">
+        <v>0.48833651612903195</v>
+      </c>
+      <c r="R44" s="49">
+        <v>0.54715942253021455</v>
+      </c>
+      <c r="S44" s="49">
+        <v>0.50726991887193296</v>
+      </c>
+      <c r="T44" s="49">
+        <v>0.47819110023041411</v>
+      </c>
+      <c r="U44" s="49">
+        <v>0.47140062225615514</v>
+      </c>
+      <c r="V44" s="49">
+        <v>0.47066835483870967</v>
+      </c>
+      <c r="W44" s="49">
+        <v>0.48476495755517823</v>
+      </c>
+      <c r="X44" s="49">
+        <v>0.50378876386936067</v>
+      </c>
+      <c r="Y44" s="49">
+        <v>0.53365469577353519</v>
+      </c>
+      <c r="Z44" s="50">
+        <v>0.58737516737508255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A46" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+      <c r="Y46" s="24"/>
+      <c r="Z46" s="24"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A47" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C47" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D47" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E47" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F47" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G47" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H47" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I47" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J47" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K47" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L47" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M47" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N47" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O47" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P47" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q47" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R47" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S47" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T47" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U47" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V47" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W47" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X47" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y47" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z47" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="49">
+        <f>B28/1000</f>
+        <v>3.3249443050516999E-3</v>
+      </c>
+      <c r="C48" s="49">
+        <f t="shared" ref="C48:Z49" si="0">C28/1000</f>
+        <v>3.6937775909186466E-3</v>
+      </c>
+      <c r="D48" s="49">
+        <f t="shared" si="0"/>
+        <v>4.8093412763626402E-3</v>
+      </c>
+      <c r="E48" s="49">
+        <f t="shared" si="0"/>
+        <v>9.2493486030175535E-3</v>
+      </c>
+      <c r="F48" s="49">
+        <f t="shared" si="0"/>
+        <v>1.2949357171222451E-2</v>
+      </c>
+      <c r="G48" s="49">
+        <f t="shared" si="0"/>
+        <v>2.0348220531654422E-2</v>
+      </c>
+      <c r="H48" s="49">
+        <f t="shared" si="0"/>
+        <v>2.9155955751745486E-2</v>
+      </c>
+      <c r="I48" s="49">
+        <f t="shared" si="0"/>
+        <v>3.8863366324139545E-2</v>
+      </c>
+      <c r="J48" s="49">
+        <f t="shared" si="0"/>
+        <v>7.1783416667577482E-2</v>
+      </c>
+      <c r="K48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11447551528397938</v>
+      </c>
+      <c r="L48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.13012707510781804</v>
+      </c>
+      <c r="M48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11417504556898904</v>
+      </c>
+      <c r="N48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11344531941092723</v>
+      </c>
+      <c r="O48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11355200000000001</v>
+      </c>
+      <c r="P48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.118254</v>
+      </c>
+      <c r="Q48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.12597320000000001</v>
+      </c>
+      <c r="R48" s="49">
+        <f>R28/1000</f>
+        <v>0.11272300000000002</v>
+      </c>
+      <c r="S48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11819280000000001</v>
+      </c>
+      <c r="T48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11080139999999999</v>
+      </c>
+      <c r="U48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11104</v>
+      </c>
+      <c r="V48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11299960000000001</v>
+      </c>
+      <c r="W48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11778444564000001</v>
+      </c>
+      <c r="X48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.11577650818400001</v>
+      </c>
+      <c r="Y48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.14137562221200001</v>
+      </c>
+      <c r="Z48" s="49">
+        <f t="shared" si="0"/>
+        <v>0.12451626466799999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="49">
+        <f>B29/1000</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E49" s="49">
+        <f t="shared" si="0"/>
+        <v>2.971001538714668E-3</v>
+      </c>
+      <c r="F49" s="49">
+        <f t="shared" si="0"/>
+        <v>2.9584970885112396E-3</v>
+      </c>
+      <c r="G49" s="49">
+        <f t="shared" si="0"/>
+        <v>5.7674712735897322E-3</v>
+      </c>
+      <c r="H49" s="49">
+        <f t="shared" si="0"/>
+        <v>7.9494199501957269E-3</v>
+      </c>
+      <c r="I49" s="49">
+        <f t="shared" si="0"/>
+        <v>7.3255835301431552E-3</v>
+      </c>
+      <c r="J49" s="49">
+        <f t="shared" si="0"/>
+        <v>1.0589388745089714E-2</v>
+      </c>
+      <c r="K49" s="49">
+        <f t="shared" si="0"/>
+        <v>7.0124062862476884E-3</v>
+      </c>
+      <c r="L49" s="49">
+        <f t="shared" si="0"/>
+        <v>6.3632262172269062E-3</v>
+      </c>
+      <c r="M49" s="49">
+        <f t="shared" si="0"/>
+        <v>8.3264514425865459E-3</v>
+      </c>
+      <c r="N49" s="49">
+        <f t="shared" si="0"/>
+        <v>1.2860989836367853E-2</v>
+      </c>
+      <c r="O49" s="49">
+        <f t="shared" si="0"/>
+        <v>5.9663487573505578E-2</v>
+      </c>
+      <c r="P49" s="49">
+        <f t="shared" si="0"/>
+        <v>7.1166463108481015E-2</v>
+      </c>
+      <c r="Q49" s="49">
+        <f t="shared" si="0"/>
+        <v>8.7889495459999925E-2</v>
+      </c>
+      <c r="R49" s="49">
+        <f>R29/1000</f>
+        <v>3.8029952380000002E-2</v>
+      </c>
+      <c r="S49" s="49">
+        <f t="shared" si="0"/>
+        <v>4.0112638132000007E-2</v>
+      </c>
+      <c r="T49" s="49">
+        <f t="shared" si="0"/>
+        <v>4.107944530999999E-2</v>
+      </c>
+      <c r="U49" s="49">
+        <f t="shared" si="0"/>
+        <v>4.6582136350000011E-2</v>
+      </c>
+      <c r="V49" s="49">
+        <f t="shared" si="0"/>
+        <v>5.4628373009999988E-2</v>
+      </c>
+      <c r="W49" s="49">
+        <f t="shared" si="0"/>
+        <v>7.0280500030000012E-2</v>
+      </c>
+      <c r="X49" s="49">
+        <f t="shared" si="0"/>
+        <v>7.0138415464000001E-2</v>
+      </c>
+      <c r="Y49" s="49">
+        <f t="shared" si="0"/>
+        <v>5.734765403999998E-2</v>
+      </c>
+      <c r="Z49" s="49">
+        <f t="shared" si="0"/>
+        <v>5.4835024290000006E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A51" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="28"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
+      <c r="Q51" s="24"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="24"/>
+      <c r="T51" s="24"/>
+      <c r="U51" s="24"/>
+      <c r="V51" s="24"/>
+      <c r="W51" s="24"/>
+      <c r="X51" s="24"/>
+      <c r="Y51" s="24"/>
+      <c r="Z51" s="24"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="42">
+        <v>1997</v>
+      </c>
+      <c r="C52" s="42">
+        <v>1998</v>
+      </c>
+      <c r="D52" s="42">
+        <v>1999</v>
+      </c>
+      <c r="E52" s="42">
+        <v>2000</v>
+      </c>
+      <c r="F52" s="42">
+        <v>2001</v>
+      </c>
+      <c r="G52" s="42">
+        <v>2002</v>
+      </c>
+      <c r="H52" s="42">
+        <v>2003</v>
+      </c>
+      <c r="I52" s="42">
+        <v>2004</v>
+      </c>
+      <c r="J52" s="42">
+        <v>2005</v>
+      </c>
+      <c r="K52" s="42">
+        <v>2006</v>
+      </c>
+      <c r="L52" s="42">
+        <v>2007</v>
+      </c>
+      <c r="M52" s="42">
+        <v>2008</v>
+      </c>
+      <c r="N52" s="42">
+        <v>2009</v>
+      </c>
+      <c r="O52" s="42">
+        <v>2010</v>
+      </c>
+      <c r="P52" s="42">
+        <v>2011</v>
+      </c>
+      <c r="Q52" s="42">
+        <v>2012</v>
+      </c>
+      <c r="R52" s="42">
+        <v>2013</v>
+      </c>
+      <c r="S52" s="42">
+        <v>2014</v>
+      </c>
+      <c r="T52" s="42">
+        <v>2015</v>
+      </c>
+      <c r="U52" s="42">
+        <v>2016</v>
+      </c>
+      <c r="V52" s="42">
+        <v>2017</v>
+      </c>
+      <c r="W52" s="43">
+        <v>2018</v>
+      </c>
+      <c r="X52" s="43">
+        <v>2019</v>
+      </c>
+      <c r="Y52" s="43">
+        <v>2020</v>
+      </c>
+      <c r="Z52" s="31">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="49">
+        <f>B33-B38-B43-B48</f>
+        <v>2.6514072580645167E-2</v>
+      </c>
+      <c r="C53" s="49">
+        <f t="shared" ref="C53:Z54" si="1">C33-C38-C43-C48</f>
+        <v>3.1394758064516123E-2</v>
+      </c>
+      <c r="D53" s="49">
+        <f t="shared" si="1"/>
+        <v>3.3988548387096751E-2</v>
+      </c>
+      <c r="E53" s="49">
+        <f t="shared" si="1"/>
+        <v>3.9072580645161295E-2</v>
+      </c>
+      <c r="F53" s="49">
+        <f t="shared" si="1"/>
+        <v>6.0815668202764961E-2</v>
+      </c>
+      <c r="G53" s="49">
+        <f t="shared" si="1"/>
+        <v>7.5649947970863662E-2</v>
+      </c>
+      <c r="H53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.10610517976116629</v>
+      </c>
+      <c r="I53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.12222233329823297</v>
+      </c>
+      <c r="J53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.16900238158432013</v>
+      </c>
+      <c r="K53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.21759223828362745</v>
+      </c>
+      <c r="L53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.28288939112903211</v>
+      </c>
+      <c r="M53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.32210593217792016</v>
+      </c>
+      <c r="N53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.35512129330943831</v>
+      </c>
+      <c r="O53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.39011801701959226</v>
+      </c>
+      <c r="P53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.42412815401258841</v>
+      </c>
+      <c r="Q53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.49672668108504414</v>
+      </c>
+      <c r="R53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.52378566605130206</v>
+      </c>
+      <c r="S53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.55582824150086929</v>
+      </c>
+      <c r="T53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.57958044354838689</v>
+      </c>
+      <c r="U53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.58687968123687728</v>
+      </c>
+      <c r="V53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.58663342741935498</v>
+      </c>
+      <c r="W53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.58534825268817203</v>
+      </c>
+      <c r="X53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.57783865709232496</v>
+      </c>
+      <c r="Y53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.58658710944700454</v>
+      </c>
+      <c r="Z53" s="49">
+        <f t="shared" si="1"/>
+        <v>0.58444901491995571</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="49">
+        <f>B34-B39-B44-B49</f>
+        <v>1.695108870967741E-2</v>
+      </c>
+      <c r="C54" s="49">
+        <f t="shared" si="1"/>
+        <v>1.7753830645161291E-2</v>
+      </c>
+      <c r="D54" s="49">
+        <f t="shared" si="1"/>
+        <v>1.9993064516129033E-2</v>
+      </c>
+      <c r="E54" s="49">
+        <f t="shared" si="1"/>
+        <v>1.7349072580645161E-2</v>
+      </c>
+      <c r="F54" s="49">
+        <f t="shared" si="1"/>
+        <v>1.8997171658986182E-2</v>
+      </c>
+      <c r="G54" s="49">
+        <f t="shared" si="1"/>
+        <v>3.0033379292403753E-2</v>
+      </c>
+      <c r="H54" s="49">
+        <f t="shared" si="1"/>
+        <v>3.7018380893300243E-2</v>
+      </c>
+      <c r="I54" s="49">
+        <f t="shared" si="1"/>
+        <v>3.8849086192726527E-2</v>
+      </c>
+      <c r="J54" s="49">
+        <f t="shared" si="1"/>
+        <v>3.0910744691710904E-2</v>
+      </c>
+      <c r="K54" s="49">
+        <f t="shared" si="1"/>
+        <v>3.3097600426049867E-2</v>
+      </c>
+      <c r="L54" s="49">
+        <f t="shared" si="1"/>
+        <v>3.3303629032258086E-2</v>
+      </c>
+      <c r="M54" s="49">
+        <f t="shared" si="1"/>
+        <v>3.7406250000000016E-2</v>
+      </c>
+      <c r="N54" s="49">
+        <f t="shared" si="1"/>
+        <v>3.9173815632476627E-2</v>
+      </c>
+      <c r="O54" s="49">
+        <f t="shared" si="1"/>
+        <v>4.3872117402132663E-2</v>
+      </c>
+      <c r="P54" s="49">
+        <f t="shared" si="1"/>
+        <v>5.1886088709677258E-2</v>
+      </c>
+      <c r="Q54" s="49">
+        <f t="shared" si="1"/>
+        <v>5.7195471616590762E-2</v>
+      </c>
+      <c r="R54" s="49">
+        <f t="shared" si="1"/>
+        <v>6.0797175034174096E-2</v>
+      </c>
+      <c r="S54" s="49">
+        <f t="shared" si="1"/>
+        <v>6.22179910814517E-2</v>
+      </c>
+      <c r="T54" s="49">
+        <f t="shared" si="1"/>
+        <v>6.6241439125190066E-2</v>
+      </c>
+      <c r="U54" s="49">
+        <f t="shared" si="1"/>
+        <v>6.5098141305892435E-2</v>
+      </c>
+      <c r="V54" s="49">
+        <f t="shared" si="1"/>
+        <v>6.9847983870967661E-2</v>
+      </c>
+      <c r="W54" s="49">
+        <f t="shared" si="1"/>
+        <v>7.0968986839717599E-2</v>
+      </c>
+      <c r="X54" s="49">
+        <f t="shared" si="1"/>
+        <v>6.4780785114919373E-2</v>
+      </c>
+      <c r="Y54" s="49">
+        <f t="shared" si="1"/>
+        <v>7.052875354536281E-2</v>
+      </c>
+      <c r="Z54" s="49">
+        <f t="shared" si="1"/>
+        <v>7.6021934867135682E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>